<commit_message>
Bringing up to date with Run 8
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_models\KModel_04\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB906AC9-B29B-4370-A160-0F1E4360750B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C2C64A-6FB4-4A3B-96A7-7F14D49B2D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -779,7 +779,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="216">
   <si>
     <t>~FI_T</t>
   </si>
@@ -1439,6 +1439,15 @@
   <si>
     <t>MIA</t>
   </si>
+  <si>
+    <t>NCAP_ILED</t>
+  </si>
+  <si>
+    <t>Delay times for construction</t>
+  </si>
+  <si>
+    <t>*ENV_ACT</t>
+  </si>
 </sst>
 </file>
 
@@ -1450,10 +1459,17 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1596,6 +1612,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1801,190 +1824,198 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="30">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="30" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="30">
+  <cellStyles count="37">
     <cellStyle name="20 % - Farve5" xfId="1" builtinId="46"/>
     <cellStyle name="20 % - Farve5 2" xfId="21" xr:uid="{A0E445DD-DB75-4F07-98F7-EA4A3CF45A39}"/>
     <cellStyle name="60 % - Farve2 2" xfId="22" xr:uid="{C9AC1626-ABF5-4D3D-AC98-65C9B7342771}"/>
@@ -1996,7 +2027,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="34" xr:uid="{BDEBB3CF-AF1C-4CB2-ABD0-D5501ABDAE80}"/>
+    <cellStyle name="Normal 2 3" xfId="33" xr:uid="{4CB49366-E867-420F-AE94-87A16FE23902}"/>
+    <cellStyle name="Normal 3" xfId="30" xr:uid="{C341F9C2-C2B1-4441-AFFB-71AB55C33019}"/>
+    <cellStyle name="Normal 3 10" xfId="35" xr:uid="{C80160CA-C69D-43F5-AB88-C0C13957D37B}"/>
+    <cellStyle name="Normal 3 2" xfId="31" xr:uid="{6ED69FBD-2431-4A2A-A985-C07F599DB5F2}"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="32" xr:uid="{458C451E-B475-47B2-B61A-A41B67973304}"/>
     <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 4 10" xfId="36" xr:uid="{E40399A7-770C-495E-95F0-22E7EBF65DC6}"/>
     <cellStyle name="Normal 4 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Normal 8" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Normal 8 2" xfId="25" xr:uid="{4EED7756-B081-4876-9BFC-75CEBE779579}"/>
@@ -2580,6 +2618,199 @@
             <a:t> is way superior to Sun01, might change in the future. </a:t>
           </a:r>
           <a:endParaRPr lang="da-DK" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>678180</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>967740</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Tekstfelt 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26CBC1E0-F88A-9BD8-B8E8-26066259BDF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8473440" y="4069080"/>
+          <a:ext cx="2758440" cy="1676400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" kern="1200"/>
+            <a:t>NCAP_ILED</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" kern="1200" baseline="0"/>
+            <a:t> added. </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="da-DK" sz="1100" kern="1200" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" kern="1200" baseline="0"/>
+            <a:t>Years based on ... pure conjecture of a google search, just to see if it works. </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="da-DK" sz="1100" kern="1200" baseline="0"/>
+          </a:br>
+          <a:br>
+            <a:rPr lang="da-DK" sz="1100" kern="1200" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" kern="1200" baseline="0"/>
+            <a:t>Should I base it on farms or individual tech..? Because if it begins building a lot, then under a year for a turbine is not realistic, but a single one doesn't take 6 years. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" kern="1200" baseline="0"/>
+            <a:t>Also based on permitting. </a:t>
+          </a:r>
+          <a:endParaRPr lang="da-DK" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Tekstfelt 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFBB1672-7AB8-89AA-2871-65714EE1B1A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12656820" y="3970020"/>
+          <a:ext cx="2255520" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" b="1" kern="1200"/>
+            <a:t>Problem with</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" b="1" kern="1200" baseline="0"/>
+            <a:t> LCOE calc here, Danish Energy Agency:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK"/>
+            <a:t>"Firstly, it mainly deals with base load technologies, i.e. power generation technologies with a relatively high number of full load hours, which is considered </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="da-DK" b="1"/>
+            <a:t>constant </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="da-DK"/>
+            <a:t>over the lifetime. It is not intended to be used for modelling and simulation of the electricity dispatch in a system with many concurrent sources."</a:t>
+          </a:r>
+          <a:endParaRPr lang="da-DK" sz="1100" kern="1200"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3487,8 +3718,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AJ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3507,15 +3738,15 @@
     <col min="13" max="14" width="14.33203125" style="22" customWidth="1"/>
     <col min="15" max="15" width="15" style="22" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2" style="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5546875" style="22" customWidth="1"/>
     <col min="18" max="18" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.77734375" customWidth="1"/>
     <col min="20" max="20" width="18.21875" customWidth="1"/>
-    <col min="21" max="21" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.33203125" customWidth="1"/>
-    <col min="23" max="23" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25" customWidth="1"/>
+    <col min="22" max="22" width="33.6640625" customWidth="1"/>
+    <col min="23" max="23" width="8.21875" customWidth="1"/>
     <col min="24" max="24" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.33203125" customWidth="1"/>
+    <col min="25" max="25" width="25.6640625" customWidth="1"/>
     <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3580,48 +3811,48 @@
       <c r="I4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="R4" s="43" t="s">
+      <c r="S4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="S4" s="43"/>
-      <c r="T4" s="44"/>
+      <c r="T4" s="43"/>
       <c r="U4" s="44"/>
       <c r="V4" s="44"/>
       <c r="W4" s="44"/>
       <c r="X4" s="44"/>
       <c r="Y4" s="44"/>
       <c r="Z4" s="44"/>
+      <c r="AA4" s="44"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="R5" s="45" t="s">
+      <c r="S5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="46" t="s">
+      <c r="T5" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="T5" s="45" t="s">
+      <c r="U5" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="45" t="s">
+      <c r="V5" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="V5" s="45" t="s">
+      <c r="W5" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="W5" s="45" t="s">
+      <c r="X5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="X5" s="45" t="s">
+      <c r="Y5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="45" t="s">
+      <c r="Z5" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="Z5" s="45" t="s">
+      <c r="AA5" s="45" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="22.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
         <v>57</v>
       </c>
@@ -3638,31 +3869,31 @@
         <v>61</v>
       </c>
       <c r="H6" s="8"/>
-      <c r="R6" s="47" t="s">
+      <c r="S6" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="S6" s="47" t="s">
+      <c r="T6" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="T6" s="47" t="s">
+      <c r="U6" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="U6" s="47" t="s">
+      <c r="V6" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="47" t="s">
+      <c r="W6" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="W6" s="47" t="s">
+      <c r="X6" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="X6" s="47" t="s">
+      <c r="Y6" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="Y6" s="47" t="s">
+      <c r="Z6" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="Z6" s="47" t="s">
+      <c r="AA6" s="47" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3683,15 +3914,15 @@
         <v>55</v>
       </c>
       <c r="H7" s="8"/>
-      <c r="R7" s="44"/>
-      <c r="S7" s="48"/>
-      <c r="T7" s="44"/>
+      <c r="S7" s="44"/>
+      <c r="T7" s="48"/>
       <c r="U7" s="44"/>
       <c r="V7" s="44"/>
       <c r="W7" s="44"/>
       <c r="X7" s="44"/>
       <c r="Y7" s="44"/>
       <c r="Z7" s="44"/>
+      <c r="AA7" s="44"/>
       <c r="AB7" s="2"/>
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
@@ -3701,7 +3932,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="5" t="s">
         <v>0</v>
       </c>
@@ -3713,7 +3944,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>1</v>
       </c>
@@ -3748,20 +3979,22 @@
         <v>71</v>
       </c>
       <c r="M11" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="N11" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="N11" s="14" t="s">
-        <v>72</v>
-      </c>
       <c r="O11" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="P11" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="Q11" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="Q11" s="24"/>
-    </row>
-    <row r="12" spans="1:36" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:36" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>74</v>
       </c>
@@ -3792,21 +4025,24 @@
         <v>115</v>
       </c>
       <c r="M12" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="N12" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="N12" s="16" t="s">
+      <c r="O12" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="O12" s="16" t="s">
+      <c r="P12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="P12" s="16" t="s">
+      <c r="Q12" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-    </row>
-    <row r="13" spans="1:36" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="1:36" ht="21.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>83</v>
       </c>
@@ -3829,31 +4065,34 @@
         <v>87</v>
       </c>
       <c r="M13" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="N13" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="N13" s="18" t="s">
+      <c r="O13" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="O13" s="18" t="s">
+      <c r="P13" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="P13" s="18"/>
-      <c r="R13" s="43" t="s">
+      <c r="Q13" s="18"/>
+      <c r="S13" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="S13" s="43"/>
-      <c r="T13" s="44"/>
+      <c r="T13" s="43"/>
       <c r="U13" s="44"/>
       <c r="V13" s="44"/>
       <c r="W13" s="44"/>
       <c r="X13" s="44"/>
       <c r="Y13" s="44"/>
       <c r="Z13" s="44"/>
+      <c r="AA13" s="44"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="str">
-        <f>T17</f>
-        <v>ELERNWSUN02</v>
+        <f>V17</f>
+        <v>Power Plants New - PV 1</v>
       </c>
       <c r="C14" s="22" t="str">
         <f>[2]Sector_Fuels_ELC!$C$20</f>
@@ -3887,43 +4126,47 @@
       <c r="L14" s="22">
         <v>25</v>
       </c>
-      <c r="O14" s="22">
+      <c r="M14" s="22">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="P14" s="22">
         <v>31.536000000000001</v>
       </c>
-      <c r="P14" s="26">
+      <c r="Q14" s="26">
         <v>1</v>
       </c>
-      <c r="R14" s="45" t="s">
+      <c r="S14" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="S14" s="46" t="s">
+      <c r="T14" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="T14" s="45" t="s">
+      <c r="U14" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="U14" s="45" t="s">
+      <c r="V14" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="V14" s="45" t="s">
+      <c r="W14" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="W14" s="45" t="s">
+      <c r="X14" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="X14" s="45" t="s">
+      <c r="Y14" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="Y14" s="45" t="s">
+      <c r="Z14" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="Z14" s="45" t="s">
+      <c r="AA14" s="45" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="21.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="str">
-        <f>T18</f>
+        <f>U18</f>
         <v>ELERNWINDOFF</v>
       </c>
       <c r="C15" s="22" t="str">
@@ -3958,43 +4201,47 @@
       <c r="L15" s="22">
         <v>25</v>
       </c>
-      <c r="O15" s="22">
+      <c r="M15" s="22">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="P15" s="22">
         <v>31.536000000000001</v>
       </c>
-      <c r="P15" s="22">
+      <c r="Q15" s="22">
         <v>1</v>
       </c>
-      <c r="R15" s="47" t="s">
+      <c r="S15" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="S15" s="47" t="s">
+      <c r="T15" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="T15" s="47" t="s">
+      <c r="U15" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="U15" s="47" t="s">
+      <c r="V15" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="V15" s="47" t="s">
+      <c r="W15" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="W15" s="47" t="s">
+      <c r="X15" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="X15" s="47" t="s">
+      <c r="Y15" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="Y15" s="47" t="s">
+      <c r="Z15" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="Z15" s="47" t="s">
+      <c r="AA15" s="47" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="str">
-        <f>T19</f>
+        <f>U19</f>
         <v>ELERNWINDON</v>
       </c>
       <c r="C16" s="22" t="str">
@@ -4030,38 +4277,42 @@
       <c r="L16" s="22">
         <v>25</v>
       </c>
-      <c r="O16" s="22">
+      <c r="M16" s="22">
+        <f>3</f>
+        <v>3</v>
+      </c>
+      <c r="P16" s="22">
         <v>31.536000000000001</v>
       </c>
-      <c r="P16" s="22">
+      <c r="Q16" s="22">
         <v>1</v>
       </c>
-      <c r="R16" s="48" t="s">
+      <c r="S16" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="S16" s="48"/>
-      <c r="T16" t="s">
+      <c r="T16" s="48"/>
+      <c r="U16" t="s">
         <v>178</v>
       </c>
-      <c r="U16" s="2" t="s">
+      <c r="V16" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>52</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>53</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>176</v>
       </c>
-      <c r="Y16" s="48"/>
       <c r="Z16" s="48"/>
-    </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA16" s="48"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="str">
-        <f>T16</f>
-        <v>ELERNWSUN01</v>
+        <f>V16</f>
+        <v>Power Plants New - PV 2</v>
       </c>
       <c r="C17" s="22" t="str">
         <f>[3]Sector_Fuels_ELC!$C$20</f>
@@ -4094,73 +4345,78 @@
       <c r="L17" s="22">
         <v>30</v>
       </c>
-      <c r="O17" s="22">
+      <c r="M17" s="22">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="P17" s="22">
         <v>31.536000000000001</v>
       </c>
-      <c r="P17" s="22">
+      <c r="Q17" s="22">
         <v>1</v>
       </c>
-      <c r="R17" s="44"/>
-      <c r="S17" s="48"/>
-      <c r="T17" t="s">
+      <c r="S17" s="44"/>
+      <c r="T17" s="48"/>
+      <c r="U17" t="s">
         <v>173</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="V17" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>52</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
         <v>53</v>
       </c>
-      <c r="X17" s="2" t="s">
+      <c r="Y17" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y17" s="48"/>
       <c r="Z17" s="48"/>
-    </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="T18" t="s">
+      <c r="AA17" s="48"/>
+    </row>
+    <row r="18" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="81"/>
+      <c r="U18" t="s">
         <v>175</v>
       </c>
-      <c r="U18" s="2" t="s">
+      <c r="V18" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>52</v>
       </c>
-      <c r="W18" t="s">
+      <c r="X18" t="s">
         <v>53</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="2:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
       <c r="J19" s="26"/>
       <c r="K19" s="26"/>
       <c r="N19" s="25"/>
       <c r="P19" s="26"/>
-      <c r="T19" s="2" t="s">
+      <c r="U19" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="U19" s="2" t="s">
+      <c r="V19" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="V19" s="2" t="s">
+      <c r="W19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="W19" s="2" t="s">
+      <c r="X19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
       <c r="J20" s="26"/>
@@ -4168,7 +4424,7 @@
       <c r="N20" s="25"/>
       <c r="P20" s="26"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="G21" s="26"/>
       <c r="N21" s="25"/>
       <c r="R21" s="48"/>
@@ -4181,21 +4437,21 @@
       <c r="Y21" s="48"/>
       <c r="Z21" s="48"/>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
       <c r="T22" s="48"/>
       <c r="U22" s="48"/>
       <c r="V22" s="48"/>
       <c r="W22" s="48"/>
       <c r="X22" s="48"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
       <c r="T23" s="48"/>
       <c r="U23" s="48"/>
       <c r="V23" s="48"/>
       <c r="W23" s="48"/>
       <c r="X23" s="48"/>
     </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
       <c r="I31" s="59" t="s">
         <v>160</v>
       </c>
@@ -4205,7 +4461,7 @@
       <c r="M31" s="60"/>
       <c r="N31" s="61"/>
     </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
       <c r="I32" s="62">
         <v>1150000</v>
       </c>
@@ -4538,14 +4794,14 @@
     </row>
     <row r="59" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I59" s="74">
-        <f>I58/O14</f>
+        <f>I58/P14</f>
         <v>2.2530641672674836</v>
       </c>
       <c r="J59" s="72" t="s">
         <v>198</v>
       </c>
       <c r="K59" s="72">
-        <f>K58/O14</f>
+        <f>K58/P14</f>
         <v>0.74277016742770163</v>
       </c>
       <c r="L59" s="72" t="s">

</xml_diff>

<commit_message>
Up to date with Run 9
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_models\KModel_04\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_04\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C2C64A-6FB4-4A3B-96A7-7F14D49B2D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E81BFBD-D50C-4779-AF4C-9F7868FBB112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3718,8 +3718,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AJ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4091,8 +4091,8 @@
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="str">
-        <f>V17</f>
-        <v>Power Plants New - PV 1</v>
+        <f>U17</f>
+        <v>ELERNWSUN02</v>
       </c>
       <c r="C14" s="22" t="str">
         <f>[2]Sector_Fuels_ELC!$C$20</f>
@@ -4311,8 +4311,8 @@
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="str">
-        <f>V16</f>
-        <v>Power Plants New - PV 2</v>
+        <f>U16</f>
+        <v>ELERNWSUN01</v>
       </c>
       <c r="C17" s="22" t="str">
         <f>[3]Sector_Fuels_ELC!$C$20</f>

</xml_diff>

<commit_message>
Up to date with model run 12
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_04\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E81BFBD-D50C-4779-AF4C-9F7868FBB112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5561BB-15AE-4BF7-9268-4B6E9088D0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -779,7 +779,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="215">
   <si>
     <t>~FI_T</t>
   </si>
@@ -1345,9 +1345,6 @@
   </si>
   <si>
     <t>Power Plants New - PV 1</t>
-  </si>
-  <si>
-    <t>Power Plants New - PV 2</t>
   </si>
   <si>
     <t>Conversions, also based on values gotten from the Teknologi kataloget</t>
@@ -3716,10 +3713,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:AJ77"/>
+  <dimension ref="A1:AL77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3979,13 +3976,13 @@
         <v>71</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N11" s="14" t="s">
         <v>174</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P11" s="14" t="s">
         <v>113</v>
@@ -4025,7 +4022,7 @@
         <v>115</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N12" s="16" t="s">
         <v>171</v>
@@ -4092,48 +4089,48 @@
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="str">
         <f>U17</f>
-        <v>ELERNWSUN02</v>
+        <v>ELERNWINDOFF</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f>[2]Sector_Fuels_ELC!$C$20</f>
-        <v>ELCSOL</v>
+        <f>[3]Sector_Fuels_ELC!$C$19</f>
+        <v>ELCWINOFF</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="22">
-        <v>2015</v>
-      </c>
-      <c r="F14" s="22">
+        <v>2020</v>
+      </c>
+      <c r="F14" s="25">
         <v>2022</v>
       </c>
       <c r="G14" s="26">
         <v>1</v>
       </c>
       <c r="H14" s="26">
-        <v>0.3</v>
+        <v>0.48</v>
       </c>
       <c r="I14" s="22">
-        <v>450</v>
-      </c>
-      <c r="J14" s="22">
-        <v>0.2</v>
+        <v>2000</v>
+      </c>
+      <c r="J14" s="26">
+        <f>I59</f>
+        <v>2.2530641672674836</v>
       </c>
       <c r="K14" s="26">
-        <f>0.5</f>
-        <v>0.5</v>
+        <v>1.19</v>
       </c>
       <c r="L14" s="22">
         <v>25</v>
       </c>
       <c r="M14" s="22">
-        <f>1</f>
-        <v>1</v>
+        <f>6</f>
+        <v>6</v>
       </c>
       <c r="P14" s="22">
         <v>31.536000000000001</v>
       </c>
-      <c r="Q14" s="26">
+      <c r="Q14" s="22">
         <v>1</v>
       </c>
       <c r="S14" s="45" t="s">
@@ -4167,11 +4164,11 @@
     <row r="15" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="str">
         <f>U18</f>
-        <v>ELERNWINDOFF</v>
+        <v>ELERNWINDON</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[3]Sector_Fuels_ELC!$C$19</f>
-        <v>ELCWINOFF</v>
+        <f>[3]Sector_Fuels_ELC!$C$18</f>
+        <v>ELCWINON</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>49</v>
@@ -4186,24 +4183,25 @@
         <v>1</v>
       </c>
       <c r="H15" s="26">
-        <v>0.48</v>
+        <v>0.35</v>
       </c>
       <c r="I15" s="22">
-        <v>2000</v>
+        <v>1200</v>
       </c>
       <c r="J15" s="26">
-        <f>I59</f>
-        <v>2.2530641672674836</v>
+        <f>K59</f>
+        <v>0.74277016742770163</v>
       </c>
       <c r="K15" s="26">
-        <v>1.19</v>
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="L15" s="22">
         <v>25</v>
       </c>
       <c r="M15" s="22">
-        <f>6</f>
-        <v>6</v>
+        <f>3</f>
+        <v>3</v>
       </c>
       <c r="P15" s="22">
         <v>31.536000000000001</v>
@@ -4241,18 +4239,18 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="str">
-        <f>U19</f>
-        <v>ELERNWINDON</v>
+        <f>U16</f>
+        <v>ELERNWSUN01</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f>[3]Sector_Fuels_ELC!$C$18</f>
-        <v>ELCWINON</v>
+        <f>[3]Sector_Fuels_ELC!$C$20</f>
+        <v>ELCSOL</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>49</v>
       </c>
       <c r="E16" s="22">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="F16" s="25">
         <v>2022</v>
@@ -4261,25 +4259,23 @@
         <v>1</v>
       </c>
       <c r="H16" s="26">
-        <v>0.35</v>
+        <v>0.12</v>
       </c>
       <c r="I16" s="22">
-        <v>1200</v>
+        <v>450</v>
       </c>
       <c r="J16" s="26">
-        <f>K59</f>
-        <v>0.74277016742770163</v>
+        <v>0.2</v>
       </c>
       <c r="K16" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="22">
+        <v>30</v>
+      </c>
+      <c r="M16" s="22">
         <f>1</f>
         <v>1</v>
-      </c>
-      <c r="L16" s="22">
-        <v>25</v>
-      </c>
-      <c r="M16" s="22">
-        <f>3</f>
-        <v>3</v>
       </c>
       <c r="P16" s="22">
         <v>31.536000000000001</v>
@@ -4295,7 +4291,7 @@
         <v>178</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="W16" t="s">
         <v>52</v>
@@ -4310,58 +4306,12 @@
       <c r="AA16" s="48"/>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="str">
-        <f>U16</f>
-        <v>ELERNWSUN01</v>
-      </c>
-      <c r="C17" s="22" t="str">
-        <f>[3]Sector_Fuels_ELC!$C$20</f>
-        <v>ELCSOL</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="22">
-        <v>2015</v>
-      </c>
-      <c r="F17" s="25">
-        <v>2022</v>
-      </c>
-      <c r="G17" s="26">
-        <v>1</v>
-      </c>
-      <c r="H17" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="I17" s="22">
-        <v>450</v>
-      </c>
-      <c r="J17" s="26">
-        <v>0.2</v>
-      </c>
-      <c r="K17" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="L17" s="22">
-        <v>30</v>
-      </c>
-      <c r="M17" s="22">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="P17" s="22">
-        <v>31.536000000000001</v>
-      </c>
-      <c r="Q17" s="22">
-        <v>1</v>
-      </c>
       <c r="S17" s="44"/>
-      <c r="T17" s="48"/>
       <c r="U17" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="W17" t="s">
         <v>52</v>
@@ -4369,24 +4319,23 @@
       <c r="X17" t="s">
         <v>53</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="Y17" t="s">
         <v>176</v>
       </c>
-      <c r="Z17" s="48"/>
       <c r="AA17" s="48"/>
     </row>
     <row r="18" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="81"/>
-      <c r="U18" t="s">
-        <v>175</v>
+      <c r="U18" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="W18" t="s">
+        <v>180</v>
+      </c>
+      <c r="W18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="X18" t="s">
+      <c r="X18" s="2" t="s">
         <v>53</v>
       </c>
       <c r="Y18" t="s">
@@ -4400,21 +4349,6 @@
       <c r="K19" s="26"/>
       <c r="N19" s="25"/>
       <c r="P19" s="26"/>
-      <c r="U19" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="V19" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="W19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="X19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="G20" s="26"/>
@@ -4473,7 +4407,7 @@
       <c r="M32" s="63"/>
       <c r="N32" s="64"/>
     </row>
-    <row r="33" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I33" s="65">
         <f>I32/10^6</f>
         <v>1.1499999999999999</v>
@@ -4486,7 +4420,7 @@
       <c r="M33" s="66"/>
       <c r="N33" s="67"/>
     </row>
-    <row r="34" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I34" s="65">
         <f>I33*1000</f>
         <v>1150</v>
@@ -4499,7 +4433,7 @@
       <c r="M34" s="66"/>
       <c r="N34" s="67"/>
     </row>
-    <row r="35" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I35" s="62">
         <v>1</v>
       </c>
@@ -4511,7 +4445,7 @@
       <c r="M35" s="63"/>
       <c r="N35" s="64"/>
     </row>
-    <row r="36" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I36" s="65">
         <f>3.6*10^-6</f>
         <v>3.5999999999999998E-6</v>
@@ -4524,7 +4458,7 @@
       <c r="M36" s="66"/>
       <c r="N36" s="67"/>
     </row>
-    <row r="37" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I37" s="65">
         <f>277777.777777777</f>
         <v>277777.777777777</v>
@@ -4537,7 +4471,7 @@
       <c r="M37" s="66"/>
       <c r="N37" s="67"/>
     </row>
-    <row r="38" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I38" s="68">
         <f>(I37*4.3)/10^6</f>
         <v>1.1944444444444411</v>
@@ -4552,7 +4486,7 @@
       <c r="M38" s="69"/>
       <c r="N38" s="70"/>
     </row>
-    <row r="39" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I39" s="62">
         <v>0.21</v>
       </c>
@@ -4564,7 +4498,7 @@
       <c r="M39" s="63"/>
       <c r="N39" s="64"/>
     </row>
-    <row r="40" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I40" s="65">
         <f>I39*1000</f>
         <v>210</v>
@@ -4577,7 +4511,7 @@
       <c r="M40" s="66"/>
       <c r="N40" s="67"/>
     </row>
-    <row r="41" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I41" s="65">
         <f>I40*1000</f>
         <v>210000</v>
@@ -4590,7 +4524,7 @@
       <c r="M41" s="66"/>
       <c r="N41" s="67"/>
     </row>
-    <row r="42" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I42" s="65">
         <f>I41*1000</f>
         <v>210000000</v>
@@ -4603,7 +4537,7 @@
       <c r="M42" s="66"/>
       <c r="N42" s="67"/>
     </row>
-    <row r="43" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I43" s="65">
         <f>I42/10^6</f>
         <v>210</v>
@@ -4616,17 +4550,83 @@
       <c r="M43" s="66"/>
       <c r="N43" s="67"/>
     </row>
-    <row r="44" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I44" s="68"/>
       <c r="J44" s="69"/>
       <c r="K44" s="69"/>
       <c r="L44" s="69"/>
       <c r="M44" s="69"/>
       <c r="N44" s="70"/>
+      <c r="W44" s="22" t="str">
+        <f>W45</f>
+        <v>ELERNWSUN02</v>
+      </c>
+      <c r="X44" s="22" t="str">
+        <f>[2]Sector_Fuels_ELC!$C$20</f>
+        <v>ELCSOL</v>
+      </c>
+      <c r="Y44" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z44" s="22">
+        <v>2015</v>
+      </c>
+      <c r="AA44" s="22">
+        <v>2022</v>
+      </c>
+      <c r="AB44" s="26">
+        <v>1</v>
+      </c>
+      <c r="AC44" s="26">
+        <v>0.3</v>
+      </c>
+      <c r="AD44" s="22">
+        <v>450</v>
+      </c>
+      <c r="AE44" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="AF44" s="26">
+        <f>0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="AG44" s="22">
+        <v>25</v>
+      </c>
+      <c r="AH44" s="22">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="AI44" s="22"/>
+      <c r="AJ44" s="22"/>
+      <c r="AK44" s="22">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="AL44" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="9:38" x14ac:dyDescent="0.25">
+      <c r="W45" t="s">
+        <v>173</v>
+      </c>
+      <c r="X45" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC45" s="48"/>
     </row>
     <row r="50" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I50" s="62" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J50" s="63"/>
       <c r="K50" s="63"/>
@@ -4638,11 +4638,11 @@
     </row>
     <row r="51" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I51" s="71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J51" s="72"/>
       <c r="K51" s="73" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L51" s="72"/>
       <c r="M51" s="72"/>
@@ -4665,7 +4665,7 @@
       </c>
       <c r="M52" s="66"/>
       <c r="N52" s="66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O52" s="66"/>
       <c r="P52" s="67"/>
@@ -4687,7 +4687,7 @@
       </c>
       <c r="M53" s="66"/>
       <c r="N53" s="66" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O53" s="66"/>
       <c r="P53" s="67"/>
@@ -4714,11 +4714,11 @@
     </row>
     <row r="55" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I55" s="71" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J55" s="72"/>
       <c r="K55" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L55" s="72"/>
       <c r="M55" s="72"/>
@@ -4732,18 +4732,18 @@
         <v>81</v>
       </c>
       <c r="J56" s="72" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K56" s="72">
         <f>23424</f>
         <v>23424</v>
       </c>
       <c r="L56" s="72" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M56" s="72"/>
       <c r="N56" s="66" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O56" s="66"/>
       <c r="P56" s="67"/>
@@ -4754,18 +4754,18 @@
         <v>71.05263157894737</v>
       </c>
       <c r="J57" s="72" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K57" s="72">
         <f>K56/10^6</f>
         <v>2.3424E-2</v>
       </c>
       <c r="L57" s="72" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M57" s="72"/>
       <c r="N57" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O57" s="66"/>
       <c r="P57" s="67"/>
@@ -4776,56 +4776,56 @@
         <v>71.05263157894737</v>
       </c>
       <c r="J58" s="72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K58" s="72">
         <f>K57*1000</f>
         <v>23.423999999999999</v>
       </c>
       <c r="L58" s="72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M58" s="72"/>
       <c r="N58" s="66" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O58" s="66"/>
       <c r="P58" s="67"/>
     </row>
     <row r="59" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I59" s="74">
-        <f>I58/P14</f>
+        <f>I58/AK44</f>
         <v>2.2530641672674836</v>
       </c>
       <c r="J59" s="72" t="s">
+        <v>197</v>
+      </c>
+      <c r="K59" s="72">
+        <f>K58/AK44</f>
+        <v>0.74277016742770163</v>
+      </c>
+      <c r="L59" s="72" t="s">
         <v>198</v>
-      </c>
-      <c r="K59" s="72">
-        <f>K58/P14</f>
-        <v>0.74277016742770163</v>
-      </c>
-      <c r="L59" s="72" t="s">
-        <v>199</v>
       </c>
       <c r="M59" s="72"/>
       <c r="N59" s="66" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O59" s="66"/>
       <c r="P59" s="67"/>
     </row>
     <row r="60" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I60" s="71" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J60" s="72"/>
       <c r="K60" s="73" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L60" s="72"/>
       <c r="M60" s="72"/>
       <c r="N60" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O60" s="72"/>
       <c r="P60" s="75">
@@ -4926,7 +4926,7 @@
         <v>164</v>
       </c>
       <c r="K68" s="66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L68" s="66"/>
       <c r="M68" s="66"/>
@@ -4936,11 +4936,11 @@
     </row>
     <row r="69" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I69" s="71" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J69" s="72"/>
       <c r="K69" s="72" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L69" s="72"/>
       <c r="M69" s="72"/>
@@ -4956,7 +4956,7 @@
         <v>166</v>
       </c>
       <c r="K70" s="66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L70" s="66"/>
       <c r="M70" s="66"/>
@@ -4973,7 +4973,7 @@
         <v>167</v>
       </c>
       <c r="K71" s="76" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L71" s="66"/>
       <c r="M71" s="66"/>
@@ -4994,11 +4994,11 @@
         <v>0.45</v>
       </c>
       <c r="L72" s="66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M72" s="66"/>
       <c r="N72" s="66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O72" s="66"/>
       <c r="P72" s="67"/>
@@ -5040,7 +5040,7 @@
     </row>
     <row r="75" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I75" s="77" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J75" s="66"/>
       <c r="K75" s="66"/>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="76" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I76" s="74" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J76" s="72"/>
       <c r="K76" s="72"/>

</xml_diff>

<commit_message>
Bringing up to date with run 17
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_04\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_models\KModel_04\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5561BB-15AE-4BF7-9268-4B6E9088D0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C950C8-DFF7-4FFD-9574-AC2CF5AF3D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -779,7 +779,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="221">
   <si>
     <t>~FI_T</t>
   </si>
@@ -1445,6 +1445,24 @@
   <si>
     <t>*ENV_ACT</t>
   </si>
+  <si>
+    <t>ELCGAS</t>
+  </si>
+  <si>
+    <t>On and offshore need to change?</t>
+  </si>
+  <si>
+    <t>Power Plants new - Natural Gas</t>
+  </si>
+  <si>
+    <t>ELCTEGAS01</t>
+  </si>
+  <si>
+    <t>M€/GW/year</t>
+  </si>
+  <si>
+    <t>OLD</t>
+  </si>
 </sst>
 </file>
 
@@ -1456,10 +1474,17 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1620,6 +1645,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1821,203 +1857,220 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="30" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="30" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="37" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="37"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="47">
     <cellStyle name="20 % - Farve5" xfId="1" builtinId="46"/>
     <cellStyle name="20 % - Farve5 2" xfId="21" xr:uid="{A0E445DD-DB75-4F07-98F7-EA4A3CF45A39}"/>
+    <cellStyle name="20 % - Farve5 3" xfId="38" xr:uid="{8A40DF18-D052-4DB8-B40C-15BAC6E6B7D7}"/>
     <cellStyle name="60 % - Farve2 2" xfId="22" xr:uid="{C9AC1626-ABF5-4D3D-AC98-65C9B7342771}"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Comma 2 2" xfId="23" xr:uid="{342F0051-E0EA-4BA9-AC78-716E2BD62BB9}"/>
+    <cellStyle name="Comma 2 2 2" xfId="45" xr:uid="{C38E6797-B183-4778-8C56-F5B4BA8A0363}"/>
+    <cellStyle name="Comma 2 3" xfId="39" xr:uid="{C9597839-C1CD-4422-9B69-09E33B80794E}"/>
     <cellStyle name="Farve2" xfId="2" builtinId="33"/>
     <cellStyle name="God" xfId="4" builtinId="26"/>
     <cellStyle name="Neutral 2" xfId="24" xr:uid="{597BBF77-CDB9-4A11-B99D-5A390083FA36}"/>
@@ -2030,11 +2083,14 @@
     <cellStyle name="Normal 3 10" xfId="35" xr:uid="{C80160CA-C69D-43F5-AB88-C0C13957D37B}"/>
     <cellStyle name="Normal 3 2" xfId="31" xr:uid="{6ED69FBD-2431-4A2A-A985-C07F599DB5F2}"/>
     <cellStyle name="Normal 3 2 2 2" xfId="32" xr:uid="{458C451E-B475-47B2-B61A-A41B67973304}"/>
+    <cellStyle name="Normal 3 3" xfId="44" xr:uid="{70A2065C-D4B2-4BDF-94FD-DC05C497DBD3}"/>
     <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 4 10" xfId="36" xr:uid="{E40399A7-770C-495E-95F0-22E7EBF65DC6}"/>
     <cellStyle name="Normal 4 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 5" xfId="37" xr:uid="{6269156B-39F7-43F5-85F4-80D26C3753BF}"/>
     <cellStyle name="Normal 8" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Normal 8 2" xfId="25" xr:uid="{4EED7756-B081-4876-9BFC-75CEBE779579}"/>
+    <cellStyle name="Normal 8 3" xfId="40" xr:uid="{05D6DDAC-C833-4036-89B1-416002114B0D}"/>
     <cellStyle name="Normal 9 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normale_B2020" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Percent 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
@@ -2042,13 +2098,17 @@
     <cellStyle name="Percent 3" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Percent 3 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Percent 3 3" xfId="27" xr:uid="{D3629B02-E58F-4590-84A7-600DFB591DC8}"/>
+    <cellStyle name="Percent 3 4" xfId="41" xr:uid="{30024190-A534-4FD1-96B2-8FC534FD5DC4}"/>
     <cellStyle name="Percent 4" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Percent 4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Percent 4 3" xfId="28" xr:uid="{4F844698-7EDB-4AC8-BFEA-F56AB7956794}"/>
+    <cellStyle name="Percent 4 4" xfId="42" xr:uid="{99D5B60D-64EC-4847-B139-DA1D2374FE39}"/>
     <cellStyle name="Percent 5" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Percent 5 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="Percent 6" xfId="29" xr:uid="{47B3D60A-936F-4AD0-8A13-3C2CAE620D29}"/>
+    <cellStyle name="Percent 7" xfId="43" xr:uid="{58FEB536-169F-4C36-BE19-F8A933DB4F32}"/>
     <cellStyle name="Procent 2" xfId="26" xr:uid="{7FEF7392-638A-4059-89E0-84FC6F34798F}"/>
+    <cellStyle name="Procent 3" xfId="46" xr:uid="{45732D75-C136-4479-B3C8-E8729918DB6F}"/>
     <cellStyle name="Standard_Sce_D_Extraction" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2293,109 +2353,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>388621</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>255271</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{006FB6B3-10AA-467C-BA1D-41E65528822C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10835641" y="7871460"/>
-          <a:ext cx="7661910" cy="335280"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>The ELCTNOIL00 can be installed from the base year to cover</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> the additional capacity needed for the reserve equation (5%)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>53340</xdr:colOff>
       <xdr:row>22</xdr:row>
@@ -2469,12 +2426,6 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t>Efficiency cannot exceed Betz limit for Wind turbines, 0.53, and is assumed slightly lower. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
             <a:rPr lang="da-DK" sz="1100"/>
             <a:t>Utilisation Factor</a:t>
           </a:r>
@@ -2496,6 +2447,15 @@
           <a:r>
             <a:rPr lang="da-DK" sz="1100" baseline="0"/>
             <a:t>ELCRNWINDOFF and ON investment cost is from the technology catalogue. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="da-DK" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" baseline="0"/>
+            <a:t>Onshore cost breakdown added in separate excel file. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2573,27 +2533,6 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t>ELCRNWSUN01 is --- </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t>ELCRNWSUN02 is --- </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t>ELCRNWIND01 is -- </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="da-DK" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
             <a:rPr lang="da-DK" sz="1100"/>
             <a:t>Variable costs added to the sun,</a:t>
           </a:r>
@@ -2601,20 +2540,6 @@
             <a:rPr lang="da-DK" sz="1100" baseline="0"/>
             <a:t> for run 9 in KModel_2</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="da-DK" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="da-DK" sz="1100"/>
-            <a:t>The Sun02</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t> is way superior to Sun01, might change in the future. </a:t>
-          </a:r>
-          <a:endParaRPr lang="da-DK" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3376,6 +3301,16 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="18">
+          <cell r="C18" t="str">
+            <v>ELCWINON</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="C19" t="str">
+            <v>ELCWINOFF</v>
+          </cell>
+        </row>
         <row r="20">
           <cell r="C20" t="str">
             <v>ELCSOL</v>
@@ -3402,16 +3337,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="18">
-          <cell r="C18" t="str">
-            <v>ELCWINON</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19" t="str">
-            <v>ELCWINOFF</v>
-          </cell>
-        </row>
         <row r="20">
           <cell r="C20" t="str">
             <v>ELCSOL</v>
@@ -3715,8 +3640,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AL77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4053,7 +3978,7 @@
         <v>84</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>85</v>
+        <v>219</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>86</v>
@@ -4092,14 +4017,14 @@
         <v>ELERNWINDOFF</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f>[3]Sector_Fuels_ELC!$C$19</f>
+        <f>[2]Sector_Fuels_ELC!$C$19</f>
         <v>ELCWINOFF</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="22">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="F14" s="25">
         <v>2022</v>
@@ -4111,21 +4036,19 @@
         <v>0.48</v>
       </c>
       <c r="I14" s="22">
-        <v>2000</v>
+        <v>1957</v>
       </c>
       <c r="J14" s="26">
-        <f>I59</f>
-        <v>2.2530641672674836</v>
+        <v>50.1</v>
       </c>
       <c r="K14" s="26">
-        <v>1.19</v>
+        <v>1.74</v>
       </c>
       <c r="L14" s="22">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="M14" s="22">
-        <f>6</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P14" s="22">
         <v>31.536000000000001</v>
@@ -4167,7 +4090,7 @@
         <v>ELERNWINDON</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[3]Sector_Fuels_ELC!$C$18</f>
+        <f>[2]Sector_Fuels_ELC!$C$18</f>
         <v>ELCWINON</v>
       </c>
       <c r="D15" s="22" t="s">
@@ -4186,22 +4109,20 @@
         <v>0.35</v>
       </c>
       <c r="I15" s="22">
-        <v>1200</v>
+        <v>1150</v>
       </c>
       <c r="J15" s="26">
-        <f>K59</f>
-        <v>0.74277016742770163</v>
+        <v>23</v>
       </c>
       <c r="K15" s="26">
-        <f>1</f>
-        <v>1</v>
+        <f>0.58</f>
+        <v>0.57999999999999996</v>
       </c>
       <c r="L15" s="22">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="M15" s="22">
-        <f>3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P15" s="22">
         <v>31.536000000000001</v>
@@ -4243,7 +4164,7 @@
         <v>ELERNWSUN01</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f>[3]Sector_Fuels_ELC!$C$20</f>
+        <f>[2]Sector_Fuels_ELC!$C$20</f>
         <v>ELCSOL</v>
       </c>
       <c r="D16" s="22" t="s">
@@ -4268,7 +4189,7 @@
         <v>0.2</v>
       </c>
       <c r="K16" s="26">
-        <v>0.5</v>
+        <v>0.06</v>
       </c>
       <c r="L16" s="22">
         <v>30</v>
@@ -4305,7 +4226,53 @@
       <c r="Z16" s="48"/>
       <c r="AA16" s="48"/>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B17" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="22">
+        <v>2020</v>
+      </c>
+      <c r="F17" s="22">
+        <v>2022</v>
+      </c>
+      <c r="G17" s="84">
+        <v>0.49</v>
+      </c>
+      <c r="H17" s="26">
+        <v>1</v>
+      </c>
+      <c r="I17" s="26">
+        <f>494.7</f>
+        <v>494.7</v>
+      </c>
+      <c r="J17" s="26">
+        <f>6.5</f>
+        <v>6.5</v>
+      </c>
+      <c r="K17" s="22">
+        <v>1.66</v>
+      </c>
+      <c r="L17" s="26">
+        <v>25</v>
+      </c>
+      <c r="M17" s="22">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="O17" s="83"/>
+      <c r="P17" s="22">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="Q17" s="22">
+        <v>1</v>
+      </c>
       <c r="S17" s="44"/>
       <c r="U17" t="s">
         <v>175</v>
@@ -4342,13 +4309,30 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="2:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
       <c r="J19" s="26"/>
       <c r="K19" s="26"/>
       <c r="N19" s="25"/>
       <c r="P19" s="26"/>
+      <c r="S19" s="85"/>
+      <c r="T19" s="85"/>
+      <c r="U19" s="82" t="s">
+        <v>218</v>
+      </c>
+      <c r="V19" s="82" t="s">
+        <v>217</v>
+      </c>
+      <c r="W19" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="X19" s="82" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y19" s="82" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="G20" s="26"/>
@@ -4360,6 +4344,9 @@
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="G21" s="26"/>
+      <c r="H21" s="22" t="s">
+        <v>216</v>
+      </c>
       <c r="N21" s="25"/>
       <c r="R21" s="48"/>
       <c r="S21" s="48"/>
@@ -4372,6 +4359,9 @@
       <c r="Z21" s="48"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="I22" s="26">
+        <v>1.19</v>
+      </c>
       <c r="T22" s="48"/>
       <c r="U22" s="48"/>
       <c r="V22" s="48"/>
@@ -4379,6 +4369,10 @@
       <c r="X22" s="48"/>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="I23" s="26">
+        <f>1</f>
+        <v>1</v>
+      </c>
       <c r="T23" s="48"/>
       <c r="U23" s="48"/>
       <c r="V23" s="48"/>
@@ -4562,7 +4556,7 @@
         <v>ELERNWSUN02</v>
       </c>
       <c r="X44" s="22" t="str">
-        <f>[2]Sector_Fuels_ELC!$C$20</f>
+        <f>[3]Sector_Fuels_ELC!$C$20</f>
         <v>ELCSOL</v>
       </c>
       <c r="Y44" s="22" t="s">
@@ -4623,6 +4617,11 @@
         <v>176</v>
       </c>
       <c r="AC45" s="48"/>
+    </row>
+    <row r="49" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I49" s="22" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="50" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I50" s="62" t="s">
@@ -4801,7 +4800,7 @@
         <v>197</v>
       </c>
       <c r="K59" s="72">
-        <f>K58/AK44</f>
+        <f>K58/P17</f>
         <v>0.74277016742770163</v>
       </c>
       <c r="L59" s="72" t="s">
@@ -6127,7 +6126,7 @@
   <dimension ref="B1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Up to date with run 21
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_models\KModel_04\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_04\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C950C8-DFF7-4FFD-9574-AC2CF5AF3D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11516DAD-34D7-4C6F-901A-54820CE95A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
@@ -779,7 +780,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="227">
   <si>
     <t>~FI_T</t>
   </si>
@@ -1326,9 +1327,6 @@
     <t>*LCOE</t>
   </si>
   <si>
-    <t>ELERNWINDOFF</t>
-  </si>
-  <si>
     <t>DAYNITE</t>
   </si>
   <si>
@@ -1338,9 +1336,6 @@
     <t>ELERNWSUN01</t>
   </si>
   <si>
-    <t>Power Plants New - Wind Offshore</t>
-  </si>
-  <si>
     <t>Power Plants New - Wind Onshore</t>
   </si>
   <si>
@@ -1443,25 +1438,49 @@
     <t>Delay times for construction</t>
   </si>
   <si>
+    <t>ELCGAS</t>
+  </si>
+  <si>
+    <t>Power Plants new - Natural Gas</t>
+  </si>
+  <si>
+    <t>ELCTEGAS01</t>
+  </si>
+  <si>
+    <t>M€/GW/year</t>
+  </si>
+  <si>
+    <t>OLD</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>ELERNWINDOFF15</t>
+  </si>
+  <si>
+    <t>ELERNWINDOFF25</t>
+  </si>
+  <si>
+    <t>ELERNWINDOFF35</t>
+  </si>
+  <si>
+    <t>ELERNWINDOFF45</t>
+  </si>
+  <si>
+    <t>Power Plants New - Wind Offshore 15 m</t>
+  </si>
+  <si>
+    <t>Power Plants New - Wind Offshore 25 m</t>
+  </si>
+  <si>
+    <t>Power Plants New - Wind Offshore 35 m</t>
+  </si>
+  <si>
+    <t>Power Plants New - Wind Offshore 45 m</t>
+  </si>
+  <si>
     <t>*ENV_ACT</t>
-  </si>
-  <si>
-    <t>ELCGAS</t>
-  </si>
-  <si>
-    <t>On and offshore need to change?</t>
-  </si>
-  <si>
-    <t>Power Plants new - Natural Gas</t>
-  </si>
-  <si>
-    <t>ELCTEGAS01</t>
-  </si>
-  <si>
-    <t>M€/GW/year</t>
-  </si>
-  <si>
-    <t>OLD</t>
   </si>
 </sst>
 </file>
@@ -1474,10 +1493,24 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1640,13 +1673,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1658,7 +1684,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1708,6 +1734,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1857,215 +1889,222 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="30" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="37" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="37"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="37" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="37"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="47"/>
+    <xf numFmtId="2" fontId="1" fillId="10" borderId="0" xfId="49" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="51">
     <cellStyle name="20 % - Farve5" xfId="1" builtinId="46"/>
     <cellStyle name="20 % - Farve5 2" xfId="21" xr:uid="{A0E445DD-DB75-4F07-98F7-EA4A3CF45A39}"/>
     <cellStyle name="20 % - Farve5 3" xfId="38" xr:uid="{8A40DF18-D052-4DB8-B40C-15BAC6E6B7D7}"/>
+    <cellStyle name="20 % - Farve5 4" xfId="48" xr:uid="{BA84CF23-2043-4E52-89AD-E947642EEB2E}"/>
+    <cellStyle name="20 % - Farve5 5" xfId="50" xr:uid="{66152348-0630-41BB-A0D0-D003EB9CAD6B}"/>
     <cellStyle name="60 % - Farve2 2" xfId="22" xr:uid="{C9AC1626-ABF5-4D3D-AC98-65C9B7342771}"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Comma 2 2" xfId="23" xr:uid="{342F0051-E0EA-4BA9-AC78-716E2BD62BB9}"/>
@@ -2088,6 +2127,8 @@
     <cellStyle name="Normal 4 10" xfId="36" xr:uid="{E40399A7-770C-495E-95F0-22E7EBF65DC6}"/>
     <cellStyle name="Normal 4 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Normal 5" xfId="37" xr:uid="{6269156B-39F7-43F5-85F4-80D26C3753BF}"/>
+    <cellStyle name="Normal 6" xfId="47" xr:uid="{7A5508E7-471B-4163-8A07-4E73C622DED6}"/>
+    <cellStyle name="Normal 7" xfId="49" xr:uid="{D3F23EFD-1EE8-4379-B78E-7BD8344176C2}"/>
     <cellStyle name="Normal 8" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Normal 8 2" xfId="25" xr:uid="{4EED7756-B081-4876-9BFC-75CEBE779579}"/>
     <cellStyle name="Normal 8 3" xfId="40" xr:uid="{05D6DDAC-C833-4036-89B1-416002114B0D}"/>
@@ -2355,13 +2396,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2548,15 +2589,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>678180</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>967740</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2571,8 +2612,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8473440" y="4069080"/>
-          <a:ext cx="2758440" cy="1676400"/>
+          <a:off x="8328660" y="3992880"/>
+          <a:ext cx="2956560" cy="2004060"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2622,7 +2663,7 @@
           </a:br>
           <a:r>
             <a:rPr lang="da-DK" sz="1100" kern="1200" baseline="0"/>
-            <a:t>Years based on ... pure conjecture of a google search, just to see if it works. </a:t>
+            <a:t>Years based on historic constructions of wind farms. pure conjecture of a google search, just to see if it works. </a:t>
           </a:r>
           <a:br>
             <a:rPr lang="da-DK" sz="1100" kern="1200" baseline="0"/>
@@ -2650,13 +2691,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3291,6 +3332,44 @@
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sector_Fuels_ELC"/>
+      <sheetName val="Con_ELC"/>
+      <sheetName val="Emi"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="19">
+          <cell r="C19" t="str">
+            <v>ELCWINOFF15</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="C20" t="str">
+            <v>ELCWINOFF25</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="C21" t="str">
+            <v>ELCWINOFF35</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="C22" t="str">
+            <v>ELCWINOFF45</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
@@ -3306,11 +3385,6 @@
             <v>ELCWINON</v>
           </cell>
         </row>
-        <row r="19">
-          <cell r="C19" t="str">
-            <v>ELCWINOFF</v>
-          </cell>
-        </row>
         <row r="20">
           <cell r="C20" t="str">
             <v>ELCSOL</v>
@@ -3324,7 +3398,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -3638,16 +3712,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:AL77"/>
+  <dimension ref="A1:AL85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="22" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="22" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" style="22" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" style="22" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" style="22" bestFit="1" customWidth="1"/>
@@ -3901,13 +3975,13 @@
         <v>71</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N11" s="14" t="s">
         <v>174</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="P11" s="14" t="s">
         <v>113</v>
@@ -3947,7 +4021,7 @@
         <v>115</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N12" s="16" t="s">
         <v>171</v>
@@ -3978,7 +4052,7 @@
         <v>84</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>86</v>
@@ -4011,14 +4085,14 @@
       <c r="Z13" s="44"/>
       <c r="AA13" s="44"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B14" s="22" t="str">
         <f>U17</f>
-        <v>ELERNWINDOFF</v>
+        <v>ELERNWINDOFF15</v>
       </c>
       <c r="C14" s="22" t="str">
         <f>[2]Sector_Fuels_ELC!$C$19</f>
-        <v>ELCWINOFF</v>
+        <v>ELCWINOFF15</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>49</v>
@@ -4035,14 +4109,14 @@
       <c r="H14" s="26">
         <v>0.48</v>
       </c>
-      <c r="I14" s="22">
-        <v>1957</v>
+      <c r="I14" s="85">
+        <v>1809.5</v>
       </c>
       <c r="J14" s="26">
-        <v>50.1</v>
-      </c>
-      <c r="K14" s="26">
-        <v>1.74</v>
+        <v>54.29</v>
+      </c>
+      <c r="K14" s="86">
+        <v>1.1399999999999999</v>
       </c>
       <c r="L14" s="22">
         <v>30</v>
@@ -4084,20 +4158,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="22" t="str">
         <f>U18</f>
-        <v>ELERNWINDON</v>
+        <v>ELERNWINDOFF25</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f>[2]Sector_Fuels_ELC!$C$18</f>
-        <v>ELCWINON</v>
+        <f>[2]Sector_Fuels_ELC!$C$20</f>
+        <v>ELCWINOFF25</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="22">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="F15" s="25">
         <v>2022</v>
@@ -4106,412 +4180,511 @@
         <v>1</v>
       </c>
       <c r="H15" s="26">
+        <v>0.48</v>
+      </c>
+      <c r="I15" s="22">
+        <v>1900</v>
+      </c>
+      <c r="J15" s="26">
+        <v>57</v>
+      </c>
+      <c r="K15" s="86">
+        <v>1.19</v>
+      </c>
+      <c r="L15" s="22">
+        <v>30</v>
+      </c>
+      <c r="M15" s="22">
+        <v>4</v>
+      </c>
+      <c r="P15" s="22">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="Q15" s="22">
+        <v>1</v>
+      </c>
+      <c r="S15" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="T15" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="U15" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="V15" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="W15" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="X15" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y15" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z15" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA15" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B16" s="22" t="str">
+        <f t="shared" ref="B16:B17" si="0">U19</f>
+        <v>ELERNWINDOFF35</v>
+      </c>
+      <c r="C16" s="22" t="str">
+        <f>[2]Sector_Fuels_ELC!$C$21</f>
+        <v>ELCWINOFF35</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="22">
+        <v>2015</v>
+      </c>
+      <c r="F16" s="25">
+        <v>2022</v>
+      </c>
+      <c r="G16" s="26">
+        <v>1</v>
+      </c>
+      <c r="H16" s="26">
+        <v>0.48</v>
+      </c>
+      <c r="I16" s="22">
+        <v>1995</v>
+      </c>
+      <c r="J16" s="26">
+        <v>59.83</v>
+      </c>
+      <c r="K16" s="86">
+        <v>1.25</v>
+      </c>
+      <c r="L16" s="22">
+        <v>30</v>
+      </c>
+      <c r="M16" s="22">
+        <v>4</v>
+      </c>
+      <c r="P16" s="22">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="Q16" s="22">
+        <v>1</v>
+      </c>
+      <c r="S16" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="T16" s="48"/>
+      <c r="U16" t="s">
+        <v>177</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="W16" t="s">
+        <v>52</v>
+      </c>
+      <c r="X16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z16" s="48"/>
+      <c r="AA16" s="48" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="2:27" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B17" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>ELERNWINDOFF45</v>
+      </c>
+      <c r="C17" s="22" t="str">
+        <f>[2]Sector_Fuels_ELC!$C$22</f>
+        <v>ELCWINOFF45</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="22">
+        <v>2015</v>
+      </c>
+      <c r="F17" s="25">
+        <v>2022</v>
+      </c>
+      <c r="G17" s="26">
+        <v>1</v>
+      </c>
+      <c r="H17" s="26">
+        <v>0.48</v>
+      </c>
+      <c r="I17" s="22">
+        <v>2071</v>
+      </c>
+      <c r="J17" s="26">
+        <v>62.1</v>
+      </c>
+      <c r="K17" s="86">
+        <v>1.29</v>
+      </c>
+      <c r="L17" s="22">
+        <v>30</v>
+      </c>
+      <c r="M17" s="22">
+        <v>4</v>
+      </c>
+      <c r="P17" s="22">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="Q17" s="22">
+        <v>1</v>
+      </c>
+      <c r="S17" s="44"/>
+      <c r="U17" t="s">
+        <v>218</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="W17" t="s">
+        <v>52</v>
+      </c>
+      <c r="X17" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA17" s="48" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B18" s="22" t="str">
+        <f>U21</f>
+        <v>ELERNWINDON</v>
+      </c>
+      <c r="C18" s="22" t="str">
+        <f>[3]Sector_Fuels_ELC!$C$18</f>
+        <v>ELCWINON</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="22">
+        <v>2020</v>
+      </c>
+      <c r="F18" s="25">
+        <v>2022</v>
+      </c>
+      <c r="G18" s="26">
+        <v>1</v>
+      </c>
+      <c r="H18" s="26">
         <v>0.35</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I18" s="22">
         <v>1150</v>
       </c>
-      <c r="J15" s="26">
+      <c r="J18" s="26">
         <v>23</v>
       </c>
-      <c r="K15" s="26">
+      <c r="K18" s="26">
+        <f>K14</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="L18" s="22">
+        <v>30</v>
+      </c>
+      <c r="M18" s="22">
+        <v>2</v>
+      </c>
+      <c r="P18" s="22">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="Q18" s="22">
+        <v>1</v>
+      </c>
+      <c r="U18" t="s">
+        <v>219</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="W18" t="s">
+        <v>52</v>
+      </c>
+      <c r="X18" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA18" s="48" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="22" t="str">
+        <f>U16</f>
+        <v>ELERNWSUN01</v>
+      </c>
+      <c r="C19" s="22" t="str">
+        <f>[3]Sector_Fuels_ELC!$C$20</f>
+        <v>ELCSOL</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="22">
+        <v>2020</v>
+      </c>
+      <c r="F19" s="25">
+        <v>2022</v>
+      </c>
+      <c r="G19" s="26">
+        <v>1</v>
+      </c>
+      <c r="H19" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="I19" s="26">
+        <f>450-J19</f>
+        <v>447</v>
+      </c>
+      <c r="J19" s="26">
+        <v>3</v>
+      </c>
+      <c r="K19" s="26"/>
+      <c r="L19" s="22">
+        <v>30</v>
+      </c>
+      <c r="M19" s="22">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="P19" s="22">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="Q19" s="22">
+        <v>1</v>
+      </c>
+      <c r="U19" t="s">
+        <v>220</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="W19" t="s">
+        <v>52</v>
+      </c>
+      <c r="X19" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA19" s="48" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B20" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="22">
+        <v>2020</v>
+      </c>
+      <c r="F20" s="22">
+        <v>2022</v>
+      </c>
+      <c r="G20" s="83">
+        <v>0.49</v>
+      </c>
+      <c r="H20" s="26">
+        <v>1</v>
+      </c>
+      <c r="I20" s="26">
+        <f>494.7</f>
+        <v>494.7</v>
+      </c>
+      <c r="J20" s="26">
+        <f>6.5</f>
+        <v>6.5</v>
+      </c>
+      <c r="K20" s="22">
+        <v>1.66</v>
+      </c>
+      <c r="L20" s="26">
+        <v>25</v>
+      </c>
+      <c r="M20" s="22">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="O20" s="82"/>
+      <c r="P20" s="22">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="Q20" s="22">
+        <v>1</v>
+      </c>
+      <c r="U20" t="s">
+        <v>221</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="W20" t="s">
+        <v>52</v>
+      </c>
+      <c r="X20" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA20" s="48" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="U21" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA21" s="48" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="U22" s="81" t="s">
+        <v>214</v>
+      </c>
+      <c r="V22" s="81" t="s">
+        <v>213</v>
+      </c>
+      <c r="W22" s="81" t="s">
+        <v>52</v>
+      </c>
+      <c r="X22" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y22" s="81" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA22" s="48" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="J24" s="22">
+        <f>(57.3-50)/3</f>
+        <v>2.4333333333333322</v>
+      </c>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="I26" s="26">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:27" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26">
+        <v>1.74</v>
+      </c>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="N27" s="25"/>
+      <c r="P27" s="26"/>
+      <c r="S27" s="84"/>
+      <c r="T27" s="84"/>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26">
+        <v>1.74</v>
+      </c>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="N28" s="25"/>
+      <c r="P28" s="26"/>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="G29" s="26"/>
+      <c r="I29" s="26">
+        <v>1.74</v>
+      </c>
+      <c r="N29" s="25"/>
+      <c r="R29" s="48"/>
+      <c r="S29" s="48"/>
+      <c r="T29" s="48"/>
+    </row>
+    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="I30" s="26">
         <f>0.58</f>
         <v>0.57999999999999996</v>
       </c>
-      <c r="L15" s="22">
-        <v>30</v>
-      </c>
-      <c r="M15" s="22">
-        <v>2</v>
-      </c>
-      <c r="P15" s="22">
-        <v>31.536000000000001</v>
-      </c>
-      <c r="Q15" s="22">
-        <v>1</v>
-      </c>
-      <c r="S15" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="T15" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="U15" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="V15" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="W15" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="X15" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y15" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z15" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA15" s="47" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="str">
-        <f>U16</f>
-        <v>ELERNWSUN01</v>
-      </c>
-      <c r="C16" s="22" t="str">
-        <f>[2]Sector_Fuels_ELC!$C$20</f>
-        <v>ELCSOL</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="22">
-        <v>2015</v>
-      </c>
-      <c r="F16" s="25">
-        <v>2022</v>
-      </c>
-      <c r="G16" s="26">
-        <v>1</v>
-      </c>
-      <c r="H16" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="I16" s="22">
-        <v>450</v>
-      </c>
-      <c r="J16" s="26">
-        <v>0.2</v>
-      </c>
-      <c r="K16" s="26">
-        <v>0.06</v>
-      </c>
-      <c r="L16" s="22">
-        <v>30</v>
-      </c>
-      <c r="M16" s="22">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="P16" s="22">
-        <v>31.536000000000001</v>
-      </c>
-      <c r="Q16" s="22">
-        <v>1</v>
-      </c>
-      <c r="S16" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="T16" s="48"/>
-      <c r="U16" t="s">
-        <v>178</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="W16" t="s">
-        <v>52</v>
-      </c>
-      <c r="X16" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z16" s="48"/>
-      <c r="AA16" s="48"/>
-    </row>
-    <row r="17" spans="2:27" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B17" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="D17" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="22">
-        <v>2020</v>
-      </c>
-      <c r="F17" s="22">
-        <v>2022</v>
-      </c>
-      <c r="G17" s="84">
-        <v>0.49</v>
-      </c>
-      <c r="H17" s="26">
-        <v>1</v>
-      </c>
-      <c r="I17" s="26">
-        <f>494.7</f>
-        <v>494.7</v>
-      </c>
-      <c r="J17" s="26">
-        <f>6.5</f>
-        <v>6.5</v>
-      </c>
-      <c r="K17" s="22">
-        <v>1.66</v>
-      </c>
-      <c r="L17" s="26">
-        <v>25</v>
-      </c>
-      <c r="M17" s="22">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="O17" s="83"/>
-      <c r="P17" s="22">
-        <v>31.536000000000001</v>
-      </c>
-      <c r="Q17" s="22">
-        <v>1</v>
-      </c>
-      <c r="S17" s="44"/>
-      <c r="U17" t="s">
-        <v>175</v>
-      </c>
-      <c r="V17" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="W17" t="s">
-        <v>52</v>
-      </c>
-      <c r="X17" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>176</v>
-      </c>
-      <c r="AA17" s="48"/>
-    </row>
-    <row r="18" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="81"/>
-      <c r="U18" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="V18" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="W18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="19" spans="2:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="N19" s="25"/>
-      <c r="P19" s="26"/>
-      <c r="S19" s="85"/>
-      <c r="T19" s="85"/>
-      <c r="U19" s="82" t="s">
-        <v>218</v>
-      </c>
-      <c r="V19" s="82" t="s">
-        <v>217</v>
-      </c>
-      <c r="W19" s="82" t="s">
-        <v>52</v>
-      </c>
-      <c r="X19" s="82" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y19" s="82" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="N20" s="25"/>
-      <c r="P20" s="26"/>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="G21" s="26"/>
-      <c r="H21" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="N21" s="25"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="48"/>
-      <c r="T21" s="48"/>
-      <c r="U21" s="48"/>
-      <c r="V21" s="48"/>
-      <c r="W21" s="48"/>
-      <c r="X21" s="44"/>
-      <c r="Y21" s="48"/>
-      <c r="Z21" s="48"/>
-    </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="I22" s="26">
-        <v>1.19</v>
-      </c>
-      <c r="T22" s="48"/>
-      <c r="U22" s="48"/>
-      <c r="V22" s="48"/>
-      <c r="W22" s="48"/>
-      <c r="X22" s="48"/>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="I23" s="26">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="T23" s="48"/>
-      <c r="U23" s="48"/>
-      <c r="V23" s="48"/>
-      <c r="W23" s="48"/>
-      <c r="X23" s="48"/>
+      <c r="T30" s="48"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="I31" s="59" t="s">
+      <c r="I31" s="26"/>
+      <c r="T31" s="48"/>
+    </row>
+    <row r="39" spans="9:38" x14ac:dyDescent="0.25">
+      <c r="I39" s="59" t="s">
         <v>160</v>
       </c>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="61"/>
-    </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="I32" s="62">
+      <c r="J39" s="60"/>
+      <c r="K39" s="60"/>
+      <c r="L39" s="60"/>
+      <c r="M39" s="60"/>
+      <c r="N39" s="61"/>
+    </row>
+    <row r="40" spans="9:38" x14ac:dyDescent="0.25">
+      <c r="I40" s="62">
         <v>1150000</v>
       </c>
-      <c r="J32" s="63" t="s">
+      <c r="J40" s="63" t="s">
         <v>159</v>
       </c>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="64"/>
-    </row>
-    <row r="33" spans="9:38" x14ac:dyDescent="0.25">
-      <c r="I33" s="65">
-        <f>I32/10^6</f>
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="J33" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="K33" s="66"/>
-      <c r="L33" s="66"/>
-      <c r="M33" s="66"/>
-      <c r="N33" s="67"/>
-    </row>
-    <row r="34" spans="9:38" x14ac:dyDescent="0.25">
-      <c r="I34" s="65">
-        <f>I33*1000</f>
-        <v>1150</v>
-      </c>
-      <c r="J34" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="K34" s="66"/>
-      <c r="L34" s="66"/>
-      <c r="M34" s="66"/>
-      <c r="N34" s="67"/>
-    </row>
-    <row r="35" spans="9:38" x14ac:dyDescent="0.25">
-      <c r="I35" s="62">
-        <v>1</v>
-      </c>
-      <c r="J35" s="63" t="s">
-        <v>161</v>
-      </c>
-      <c r="K35" s="63"/>
-      <c r="L35" s="63"/>
-      <c r="M35" s="63"/>
-      <c r="N35" s="64"/>
-    </row>
-    <row r="36" spans="9:38" x14ac:dyDescent="0.25">
-      <c r="I36" s="65">
-        <f>3.6*10^-6</f>
-        <v>3.5999999999999998E-6</v>
-      </c>
-      <c r="J36" s="66" t="s">
-        <v>163</v>
-      </c>
-      <c r="K36" s="66"/>
-      <c r="L36" s="66"/>
-      <c r="M36" s="66"/>
-      <c r="N36" s="67"/>
-    </row>
-    <row r="37" spans="9:38" x14ac:dyDescent="0.25">
-      <c r="I37" s="65">
-        <f>277777.777777777</f>
-        <v>277777.777777777</v>
-      </c>
-      <c r="J37" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="K37" s="66"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="66"/>
-      <c r="N37" s="67"/>
-    </row>
-    <row r="38" spans="9:38" x14ac:dyDescent="0.25">
-      <c r="I38" s="68">
-        <f>(I37*4.3)/10^6</f>
-        <v>1.1944444444444411</v>
-      </c>
-      <c r="J38" s="69" t="s">
-        <v>164</v>
-      </c>
-      <c r="K38" s="69" t="s">
-        <v>165</v>
-      </c>
-      <c r="L38" s="69"/>
-      <c r="M38" s="69"/>
-      <c r="N38" s="70"/>
-    </row>
-    <row r="39" spans="9:38" x14ac:dyDescent="0.25">
-      <c r="I39" s="62">
-        <v>0.21</v>
-      </c>
-      <c r="J39" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="K39" s="63"/>
-      <c r="L39" s="63"/>
-      <c r="M39" s="63"/>
-      <c r="N39" s="64"/>
-    </row>
-    <row r="40" spans="9:38" x14ac:dyDescent="0.25">
-      <c r="I40" s="65">
-        <f>I39*1000</f>
-        <v>210</v>
-      </c>
-      <c r="J40" s="66" t="s">
-        <v>167</v>
-      </c>
-      <c r="K40" s="66"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="66"/>
-      <c r="N40" s="67"/>
+      <c r="K40" s="63"/>
+      <c r="L40" s="63"/>
+      <c r="M40" s="63"/>
+      <c r="N40" s="64"/>
     </row>
     <row r="41" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I41" s="65">
-        <f>I40*1000</f>
-        <v>210000</v>
+        <f>I40/10^6</f>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J41" s="66" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="K41" s="66"/>
       <c r="L41" s="66"/>
@@ -4521,10 +4694,10 @@
     <row r="42" spans="9:38" x14ac:dyDescent="0.25">
       <c r="I42" s="65">
         <f>I41*1000</f>
-        <v>210000000</v>
+        <v>1150</v>
       </c>
       <c r="J42" s="66" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="K42" s="66"/>
       <c r="L42" s="66"/>
@@ -4532,31 +4705,35 @@
       <c r="N42" s="67"/>
     </row>
     <row r="43" spans="9:38" x14ac:dyDescent="0.25">
-      <c r="I43" s="65">
-        <f>I42/10^6</f>
-        <v>210</v>
-      </c>
-      <c r="J43" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="K43" s="66"/>
-      <c r="L43" s="66"/>
-      <c r="M43" s="66"/>
-      <c r="N43" s="67"/>
+      <c r="I43" s="62">
+        <v>1</v>
+      </c>
+      <c r="J43" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="64"/>
     </row>
     <row r="44" spans="9:38" x14ac:dyDescent="0.25">
-      <c r="I44" s="68"/>
-      <c r="J44" s="69"/>
-      <c r="K44" s="69"/>
-      <c r="L44" s="69"/>
-      <c r="M44" s="69"/>
-      <c r="N44" s="70"/>
+      <c r="I44" s="65">
+        <f>3.6*10^-6</f>
+        <v>3.5999999999999998E-6</v>
+      </c>
+      <c r="J44" s="66" t="s">
+        <v>163</v>
+      </c>
+      <c r="K44" s="66"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="66"/>
+      <c r="N44" s="67"/>
       <c r="W44" s="22" t="str">
         <f>W45</f>
         <v>ELERNWSUN02</v>
       </c>
       <c r="X44" s="22" t="str">
-        <f>[3]Sector_Fuels_ELC!$C$20</f>
+        <f>[4]Sector_Fuels_ELC!$C$20</f>
         <v>ELCSOL</v>
       </c>
       <c r="Y44" s="22" t="s">
@@ -4601,11 +4778,22 @@
       </c>
     </row>
     <row r="45" spans="9:38" x14ac:dyDescent="0.25">
+      <c r="I45" s="65">
+        <f>277777.777777777</f>
+        <v>277777.777777777</v>
+      </c>
+      <c r="J45" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="K45" s="66"/>
+      <c r="L45" s="66"/>
+      <c r="M45" s="66"/>
+      <c r="N45" s="67"/>
       <c r="W45" t="s">
         <v>173</v>
       </c>
       <c r="X45" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Y45" t="s">
         <v>52</v>
@@ -4614,333 +4802,315 @@
         <v>53</v>
       </c>
       <c r="AA45" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AC45" s="48"/>
     </row>
+    <row r="46" spans="9:38" x14ac:dyDescent="0.25">
+      <c r="I46" s="68">
+        <f>(I45*4.3)/10^6</f>
+        <v>1.1944444444444411</v>
+      </c>
+      <c r="J46" s="69" t="s">
+        <v>164</v>
+      </c>
+      <c r="K46" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="L46" s="69"/>
+      <c r="M46" s="69"/>
+      <c r="N46" s="70"/>
+    </row>
+    <row r="47" spans="9:38" x14ac:dyDescent="0.25">
+      <c r="I47" s="62">
+        <v>0.21</v>
+      </c>
+      <c r="J47" s="63" t="s">
+        <v>166</v>
+      </c>
+      <c r="K47" s="63"/>
+      <c r="L47" s="63"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="64"/>
+    </row>
+    <row r="48" spans="9:38" x14ac:dyDescent="0.25">
+      <c r="I48" s="65">
+        <f>I47*1000</f>
+        <v>210</v>
+      </c>
+      <c r="J48" s="66" t="s">
+        <v>167</v>
+      </c>
+      <c r="K48" s="66"/>
+      <c r="L48" s="66"/>
+      <c r="M48" s="66"/>
+      <c r="N48" s="67"/>
+    </row>
     <row r="49" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I49" s="22" t="s">
-        <v>220</v>
-      </c>
+      <c r="I49" s="65">
+        <f>I48*1000</f>
+        <v>210000</v>
+      </c>
+      <c r="J49" s="66" t="s">
+        <v>168</v>
+      </c>
+      <c r="K49" s="66"/>
+      <c r="L49" s="66"/>
+      <c r="M49" s="66"/>
+      <c r="N49" s="67"/>
     </row>
     <row r="50" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I50" s="62" t="s">
+      <c r="I50" s="65">
+        <f>I49*1000</f>
+        <v>210000000</v>
+      </c>
+      <c r="J50" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="K50" s="66"/>
+      <c r="L50" s="66"/>
+      <c r="M50" s="66"/>
+      <c r="N50" s="67"/>
+    </row>
+    <row r="51" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I51" s="65">
+        <f>I50/10^6</f>
+        <v>210</v>
+      </c>
+      <c r="J51" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="K51" s="66"/>
+      <c r="L51" s="66"/>
+      <c r="M51" s="66"/>
+      <c r="N51" s="67"/>
+    </row>
+    <row r="52" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I52" s="68"/>
+      <c r="J52" s="69"/>
+      <c r="K52" s="69"/>
+      <c r="L52" s="69"/>
+      <c r="M52" s="69"/>
+      <c r="N52" s="70"/>
+    </row>
+    <row r="57" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I57" s="22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I58" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="J58" s="63"/>
+      <c r="K58" s="63"/>
+      <c r="L58" s="63"/>
+      <c r="M58" s="63"/>
+      <c r="N58" s="63"/>
+      <c r="O58" s="63"/>
+      <c r="P58" s="64"/>
+    </row>
+    <row r="59" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="I59" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="J59" s="72"/>
+      <c r="K59" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="J50" s="63"/>
-      <c r="K50" s="63"/>
-      <c r="L50" s="63"/>
-      <c r="M50" s="63"/>
-      <c r="N50" s="63"/>
-      <c r="O50" s="63"/>
-      <c r="P50" s="64"/>
-    </row>
-    <row r="51" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="I51" s="71" t="s">
+      <c r="L59" s="72"/>
+      <c r="M59" s="72"/>
+      <c r="N59" s="66"/>
+      <c r="O59" s="66"/>
+      <c r="P59" s="67"/>
+    </row>
+    <row r="60" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I60" s="65">
+        <v>2000000</v>
+      </c>
+      <c r="J60" s="66" t="s">
+        <v>159</v>
+      </c>
+      <c r="K60" s="65">
+        <v>1200000</v>
+      </c>
+      <c r="L60" s="66" t="s">
+        <v>159</v>
+      </c>
+      <c r="M60" s="66"/>
+      <c r="N60" s="66" t="s">
         <v>183</v>
       </c>
-      <c r="J51" s="72"/>
-      <c r="K51" s="73" t="s">
+      <c r="O60" s="66"/>
+      <c r="P60" s="67"/>
+    </row>
+    <row r="61" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I61" s="65">
+        <f>I60/10^6</f>
+        <v>2</v>
+      </c>
+      <c r="J61" s="66" t="s">
+        <v>157</v>
+      </c>
+      <c r="K61" s="65">
+        <f>K60/10^6</f>
+        <v>1.2</v>
+      </c>
+      <c r="L61" s="66" t="s">
+        <v>157</v>
+      </c>
+      <c r="M61" s="66"/>
+      <c r="N61" s="66" t="s">
         <v>184</v>
       </c>
-      <c r="L51" s="72"/>
-      <c r="M51" s="72"/>
-      <c r="N51" s="66"/>
-      <c r="O51" s="66"/>
-      <c r="P51" s="67"/>
-    </row>
-    <row r="52" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I52" s="65">
-        <v>2000000</v>
-      </c>
-      <c r="J52" s="66" t="s">
-        <v>159</v>
-      </c>
-      <c r="K52" s="65">
-        <v>1200000</v>
-      </c>
-      <c r="L52" s="66" t="s">
-        <v>159</v>
-      </c>
-      <c r="M52" s="66"/>
-      <c r="N52" s="66" t="s">
+      <c r="O61" s="66"/>
+      <c r="P61" s="67"/>
+    </row>
+    <row r="62" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I62" s="65">
+        <f>I61*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="J62" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="K62" s="65">
+        <f>K61*1000</f>
+        <v>1200</v>
+      </c>
+      <c r="L62" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="M62" s="66"/>
+      <c r="N62" s="66"/>
+      <c r="O62" s="66"/>
+      <c r="P62" s="67"/>
+    </row>
+    <row r="63" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="I63" s="71" t="s">
         <v>185</v>
       </c>
-      <c r="O52" s="66"/>
-      <c r="P52" s="67"/>
-    </row>
-    <row r="53" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I53" s="65">
-        <f>I52/10^6</f>
-        <v>2</v>
-      </c>
-      <c r="J53" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="K53" s="65">
-        <f>K52/10^6</f>
-        <v>1.2</v>
-      </c>
-      <c r="L53" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="M53" s="66"/>
-      <c r="N53" s="66" t="s">
+      <c r="J63" s="72"/>
+      <c r="K63" s="73" t="s">
         <v>186</v>
       </c>
-      <c r="O53" s="66"/>
-      <c r="P53" s="67"/>
-    </row>
-    <row r="54" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I54" s="65">
-        <f>I53*1000</f>
-        <v>2000</v>
-      </c>
-      <c r="J54" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="K54" s="65">
-        <f>K53*1000</f>
-        <v>1200</v>
-      </c>
-      <c r="L54" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="M54" s="66"/>
-      <c r="N54" s="66"/>
-      <c r="O54" s="66"/>
-      <c r="P54" s="67"/>
-    </row>
-    <row r="55" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="I55" s="71" t="s">
-        <v>187</v>
-      </c>
-      <c r="J55" s="72"/>
-      <c r="K55" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="L55" s="72"/>
-      <c r="M55" s="72"/>
-      <c r="N55" s="66"/>
-      <c r="O55" s="66"/>
-      <c r="P55" s="67"/>
-    </row>
-    <row r="56" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I56" s="74">
+      <c r="L63" s="72"/>
+      <c r="M63" s="72"/>
+      <c r="N63" s="66"/>
+      <c r="O63" s="66"/>
+      <c r="P63" s="67"/>
+    </row>
+    <row r="64" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I64" s="74">
         <f>81</f>
         <v>81</v>
       </c>
-      <c r="J56" s="72" t="s">
-        <v>189</v>
-      </c>
-      <c r="K56" s="72">
+      <c r="J64" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="K64" s="72">
         <f>23424</f>
         <v>23424</v>
       </c>
-      <c r="L56" s="72" t="s">
+      <c r="L64" s="72" t="s">
+        <v>188</v>
+      </c>
+      <c r="M64" s="72"/>
+      <c r="N64" s="66" t="s">
+        <v>189</v>
+      </c>
+      <c r="O64" s="66"/>
+      <c r="P64" s="67"/>
+    </row>
+    <row r="65" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I65" s="74">
+        <f>I64/P68</f>
+        <v>71.05263157894737</v>
+      </c>
+      <c r="J65" s="72" t="s">
         <v>190</v>
       </c>
-      <c r="M56" s="72"/>
-      <c r="N56" s="66" t="s">
+      <c r="K65" s="72">
+        <f>K64/10^6</f>
+        <v>2.3424E-2</v>
+      </c>
+      <c r="L65" s="72" t="s">
         <v>191</v>
       </c>
-      <c r="O56" s="66"/>
-      <c r="P56" s="67"/>
-    </row>
-    <row r="57" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I57" s="74">
-        <f>I56/P60</f>
+      <c r="M65" s="72"/>
+      <c r="N65" s="66" t="s">
+        <v>192</v>
+      </c>
+      <c r="O65" s="66"/>
+      <c r="P65" s="67"/>
+    </row>
+    <row r="66" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I66" s="74">
+        <f>(I65*1000000)/10^6</f>
         <v>71.05263157894737</v>
       </c>
-      <c r="J57" s="72" t="s">
-        <v>192</v>
-      </c>
-      <c r="K57" s="72">
-        <f>K56/10^6</f>
-        <v>2.3424E-2</v>
-      </c>
-      <c r="L57" s="72" t="s">
+      <c r="J66" s="72" t="s">
         <v>193</v>
       </c>
-      <c r="M57" s="72"/>
-      <c r="N57" s="66" t="s">
+      <c r="K66" s="72">
+        <f>K65*1000</f>
+        <v>23.423999999999999</v>
+      </c>
+      <c r="L66" s="72" t="s">
+        <v>193</v>
+      </c>
+      <c r="M66" s="72"/>
+      <c r="N66" s="66" t="s">
         <v>194</v>
       </c>
-      <c r="O57" s="66"/>
-      <c r="P57" s="67"/>
-    </row>
-    <row r="58" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I58" s="74">
-        <f>(I57*1000000)/10^6</f>
-        <v>71.05263157894737</v>
-      </c>
-      <c r="J58" s="72" t="s">
+      <c r="O66" s="66"/>
+      <c r="P66" s="67"/>
+    </row>
+    <row r="67" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I67" s="74">
+        <f>I66/AK44</f>
+        <v>2.2530641672674836</v>
+      </c>
+      <c r="J67" s="72" t="s">
         <v>195</v>
       </c>
-      <c r="K58" s="72">
-        <f>K57*1000</f>
-        <v>23.423999999999999</v>
-      </c>
-      <c r="L58" s="72" t="s">
-        <v>195</v>
-      </c>
-      <c r="M58" s="72"/>
-      <c r="N58" s="66" t="s">
+      <c r="K67" s="72">
+        <f>K66/P20</f>
+        <v>0.74277016742770163</v>
+      </c>
+      <c r="L67" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="O58" s="66"/>
-      <c r="P58" s="67"/>
-    </row>
-    <row r="59" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I59" s="74">
-        <f>I58/AK44</f>
-        <v>2.2530641672674836</v>
-      </c>
-      <c r="J59" s="72" t="s">
+      <c r="M67" s="72"/>
+      <c r="N67" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="K59" s="72">
-        <f>K58/P17</f>
-        <v>0.74277016742770163</v>
-      </c>
-      <c r="L59" s="72" t="s">
+      <c r="O67" s="66"/>
+      <c r="P67" s="67"/>
+    </row>
+    <row r="68" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="I68" s="71" t="s">
         <v>198</v>
       </c>
-      <c r="M59" s="72"/>
-      <c r="N59" s="66" t="s">
+      <c r="J68" s="72"/>
+      <c r="K68" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="O59" s="66"/>
-      <c r="P59" s="67"/>
-    </row>
-    <row r="60" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="I60" s="71" t="s">
+      <c r="L68" s="72"/>
+      <c r="M68" s="72"/>
+      <c r="N68" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="J60" s="72"/>
-      <c r="K60" s="73" t="s">
-        <v>201</v>
-      </c>
-      <c r="L60" s="72"/>
-      <c r="M60" s="72"/>
-      <c r="N60" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="O60" s="72"/>
-      <c r="P60" s="75">
+      <c r="O68" s="72"/>
+      <c r="P68" s="75">
         <f>1.14</f>
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="61" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I61" s="74"/>
-      <c r="J61" s="72"/>
-      <c r="K61" s="72"/>
-      <c r="L61" s="72"/>
-      <c r="M61" s="72"/>
-      <c r="N61" s="72"/>
-      <c r="O61" s="72"/>
-      <c r="P61" s="75"/>
-    </row>
-    <row r="62" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I62" s="74"/>
-      <c r="J62" s="72"/>
-      <c r="K62" s="72"/>
-      <c r="L62" s="72"/>
-      <c r="M62" s="72"/>
-      <c r="N62" s="72"/>
-      <c r="O62" s="72"/>
-      <c r="P62" s="75"/>
-    </row>
-    <row r="63" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I63" s="74"/>
-      <c r="J63" s="72"/>
-      <c r="K63" s="72"/>
-      <c r="L63" s="72"/>
-      <c r="M63" s="72"/>
-      <c r="N63" s="72"/>
-      <c r="O63" s="72"/>
-      <c r="P63" s="75"/>
-    </row>
-    <row r="64" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I64" s="74"/>
-      <c r="J64" s="72"/>
-      <c r="K64" s="72"/>
-      <c r="L64" s="72"/>
-      <c r="M64" s="72"/>
-      <c r="N64" s="72"/>
-      <c r="O64" s="72"/>
-      <c r="P64" s="75"/>
-    </row>
-    <row r="65" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I65" s="65">
-        <v>1</v>
-      </c>
-      <c r="J65" s="66" t="s">
-        <v>161</v>
-      </c>
-      <c r="K65" s="66"/>
-      <c r="L65" s="66"/>
-      <c r="M65" s="66"/>
-      <c r="N65" s="66"/>
-      <c r="O65" s="66"/>
-      <c r="P65" s="67"/>
-    </row>
-    <row r="66" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I66" s="65">
-        <f>3.6*10^-6</f>
-        <v>3.5999999999999998E-6</v>
-      </c>
-      <c r="J66" s="66" t="s">
-        <v>163</v>
-      </c>
-      <c r="K66" s="66"/>
-      <c r="L66" s="66"/>
-      <c r="M66" s="66"/>
-      <c r="N66" s="66"/>
-      <c r="O66" s="66"/>
-      <c r="P66" s="67"/>
-    </row>
-    <row r="67" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I67" s="65">
-        <f>277777.777777777</f>
-        <v>277777.777777777</v>
-      </c>
-      <c r="J67" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="K67" s="66"/>
-      <c r="L67" s="66"/>
-      <c r="M67" s="66"/>
-      <c r="N67" s="66"/>
-      <c r="O67" s="66"/>
-      <c r="P67" s="67"/>
-    </row>
-    <row r="68" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I68" s="65">
-        <f>(I67*4.3)/10^6</f>
-        <v>1.1944444444444411</v>
-      </c>
-      <c r="J68" s="66" t="s">
-        <v>164</v>
-      </c>
-      <c r="K68" s="66" t="s">
-        <v>203</v>
-      </c>
-      <c r="L68" s="66"/>
-      <c r="M68" s="66"/>
-      <c r="N68" s="66"/>
-      <c r="O68" s="66"/>
-      <c r="P68" s="67"/>
-    </row>
-    <row r="69" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="I69" s="71" t="s">
-        <v>204</v>
-      </c>
+    <row r="69" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I69" s="74"/>
       <c r="J69" s="72"/>
-      <c r="K69" s="72" t="s">
-        <v>205</v>
-      </c>
+      <c r="K69" s="72"/>
       <c r="L69" s="72"/>
       <c r="M69" s="72"/>
       <c r="N69" s="72"/>
@@ -4948,75 +5118,44 @@
       <c r="P69" s="75"/>
     </row>
     <row r="70" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I70" s="65">
-        <v>0.21</v>
-      </c>
-      <c r="J70" s="66" t="s">
-        <v>166</v>
-      </c>
-      <c r="K70" s="66" t="s">
-        <v>206</v>
-      </c>
-      <c r="L70" s="66"/>
-      <c r="M70" s="66"/>
-      <c r="N70" s="66"/>
-      <c r="O70" s="66"/>
-      <c r="P70" s="67"/>
+      <c r="I70" s="74"/>
+      <c r="J70" s="72"/>
+      <c r="K70" s="72"/>
+      <c r="L70" s="72"/>
+      <c r="M70" s="72"/>
+      <c r="N70" s="72"/>
+      <c r="O70" s="72"/>
+      <c r="P70" s="75"/>
     </row>
     <row r="71" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I71" s="65">
-        <f>I70*1000</f>
-        <v>210</v>
-      </c>
-      <c r="J71" s="66" t="s">
-        <v>167</v>
-      </c>
-      <c r="K71" s="76" t="s">
-        <v>207</v>
-      </c>
-      <c r="L71" s="66"/>
-      <c r="M71" s="66"/>
-      <c r="N71" s="66"/>
-      <c r="O71" s="66"/>
-      <c r="P71" s="67"/>
+      <c r="I71" s="74"/>
+      <c r="J71" s="72"/>
+      <c r="K71" s="72"/>
+      <c r="L71" s="72"/>
+      <c r="M71" s="72"/>
+      <c r="N71" s="72"/>
+      <c r="O71" s="72"/>
+      <c r="P71" s="75"/>
     </row>
     <row r="72" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I72" s="65">
-        <f>I71*1000</f>
-        <v>210000</v>
-      </c>
-      <c r="J72" s="66" t="s">
-        <v>168</v>
-      </c>
-      <c r="K72" s="66">
-        <f>0.45</f>
-        <v>0.45</v>
-      </c>
-      <c r="L72" s="66" t="s">
-        <v>208</v>
-      </c>
-      <c r="M72" s="66"/>
-      <c r="N72" s="66" t="s">
-        <v>209</v>
-      </c>
-      <c r="O72" s="66"/>
-      <c r="P72" s="67"/>
+      <c r="I72" s="74"/>
+      <c r="J72" s="72"/>
+      <c r="K72" s="72"/>
+      <c r="L72" s="72"/>
+      <c r="M72" s="72"/>
+      <c r="N72" s="72"/>
+      <c r="O72" s="72"/>
+      <c r="P72" s="75"/>
     </row>
     <row r="73" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I73" s="65">
-        <f>I72*1000</f>
-        <v>210000000</v>
+        <v>1</v>
       </c>
       <c r="J73" s="66" t="s">
-        <v>169</v>
-      </c>
-      <c r="K73" s="66">
-        <f>K72*1000</f>
-        <v>450</v>
-      </c>
-      <c r="L73" s="66" t="s">
-        <v>170</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="K73" s="66"/>
+      <c r="L73" s="66"/>
       <c r="M73" s="66"/>
       <c r="N73" s="66"/>
       <c r="O73" s="66"/>
@@ -5024,11 +5163,11 @@
     </row>
     <row r="74" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I74" s="65">
-        <f>I73/10^6</f>
-        <v>210</v>
+        <f>3.6*10^-6</f>
+        <v>3.5999999999999998E-6</v>
       </c>
       <c r="J74" s="66" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="K74" s="66"/>
       <c r="L74" s="66"/>
@@ -5038,10 +5177,13 @@
       <c r="P74" s="67"/>
     </row>
     <row r="75" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I75" s="77" t="s">
-        <v>210</v>
-      </c>
-      <c r="J75" s="66"/>
+      <c r="I75" s="65">
+        <f>277777.777777777</f>
+        <v>277777.777777777</v>
+      </c>
+      <c r="J75" s="66" t="s">
+        <v>162</v>
+      </c>
       <c r="K75" s="66"/>
       <c r="L75" s="66"/>
       <c r="M75" s="66"/>
@@ -5050,26 +5192,159 @@
       <c r="P75" s="67"/>
     </row>
     <row r="76" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I76" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="J76" s="72"/>
-      <c r="K76" s="72"/>
-      <c r="L76" s="72"/>
-      <c r="M76" s="72"/>
-      <c r="N76" s="72"/>
-      <c r="O76" s="72"/>
-      <c r="P76" s="75"/>
-    </row>
-    <row r="77" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I77" s="78"/>
-      <c r="J77" s="79"/>
-      <c r="K77" s="79"/>
-      <c r="L77" s="79"/>
-      <c r="M77" s="79"/>
-      <c r="N77" s="79"/>
-      <c r="O77" s="79"/>
-      <c r="P77" s="80"/>
+      <c r="I76" s="65">
+        <f>(I75*4.3)/10^6</f>
+        <v>1.1944444444444411</v>
+      </c>
+      <c r="J76" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="K76" s="66" t="s">
+        <v>201</v>
+      </c>
+      <c r="L76" s="66"/>
+      <c r="M76" s="66"/>
+      <c r="N76" s="66"/>
+      <c r="O76" s="66"/>
+      <c r="P76" s="67"/>
+    </row>
+    <row r="77" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="I77" s="71" t="s">
+        <v>202</v>
+      </c>
+      <c r="J77" s="72"/>
+      <c r="K77" s="72" t="s">
+        <v>203</v>
+      </c>
+      <c r="L77" s="72"/>
+      <c r="M77" s="72"/>
+      <c r="N77" s="72"/>
+      <c r="O77" s="72"/>
+      <c r="P77" s="75"/>
+    </row>
+    <row r="78" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I78" s="65">
+        <v>0.21</v>
+      </c>
+      <c r="J78" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="K78" s="66" t="s">
+        <v>204</v>
+      </c>
+      <c r="L78" s="66"/>
+      <c r="M78" s="66"/>
+      <c r="N78" s="66"/>
+      <c r="O78" s="66"/>
+      <c r="P78" s="67"/>
+    </row>
+    <row r="79" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I79" s="65">
+        <f>I78*1000</f>
+        <v>210</v>
+      </c>
+      <c r="J79" s="66" t="s">
+        <v>167</v>
+      </c>
+      <c r="K79" s="76" t="s">
+        <v>205</v>
+      </c>
+      <c r="L79" s="66"/>
+      <c r="M79" s="66"/>
+      <c r="N79" s="66"/>
+      <c r="O79" s="66"/>
+      <c r="P79" s="67"/>
+    </row>
+    <row r="80" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I80" s="65">
+        <f>I79*1000</f>
+        <v>210000</v>
+      </c>
+      <c r="J80" s="66" t="s">
+        <v>168</v>
+      </c>
+      <c r="K80" s="66">
+        <f>0.45</f>
+        <v>0.45</v>
+      </c>
+      <c r="L80" s="66" t="s">
+        <v>206</v>
+      </c>
+      <c r="M80" s="66"/>
+      <c r="N80" s="66" t="s">
+        <v>207</v>
+      </c>
+      <c r="O80" s="66"/>
+      <c r="P80" s="67"/>
+    </row>
+    <row r="81" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I81" s="65">
+        <f>I80*1000</f>
+        <v>210000000</v>
+      </c>
+      <c r="J81" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="K81" s="66">
+        <f>K80*1000</f>
+        <v>450</v>
+      </c>
+      <c r="L81" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="M81" s="66"/>
+      <c r="N81" s="66"/>
+      <c r="O81" s="66"/>
+      <c r="P81" s="67"/>
+    </row>
+    <row r="82" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I82" s="65">
+        <f>I81/10^6</f>
+        <v>210</v>
+      </c>
+      <c r="J82" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="K82" s="66"/>
+      <c r="L82" s="66"/>
+      <c r="M82" s="66"/>
+      <c r="N82" s="66"/>
+      <c r="O82" s="66"/>
+      <c r="P82" s="67"/>
+    </row>
+    <row r="83" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I83" s="77" t="s">
+        <v>208</v>
+      </c>
+      <c r="J83" s="66"/>
+      <c r="K83" s="66"/>
+      <c r="L83" s="66"/>
+      <c r="M83" s="66"/>
+      <c r="N83" s="66"/>
+      <c r="O83" s="66"/>
+      <c r="P83" s="67"/>
+    </row>
+    <row r="84" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I84" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="J84" s="72"/>
+      <c r="K84" s="72"/>
+      <c r="L84" s="72"/>
+      <c r="M84" s="72"/>
+      <c r="N84" s="72"/>
+      <c r="O84" s="72"/>
+      <c r="P84" s="75"/>
+    </row>
+    <row r="85" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I85" s="78"/>
+      <c r="J85" s="79"/>
+      <c r="K85" s="79"/>
+      <c r="L85" s="79"/>
+      <c r="M85" s="79"/>
+      <c r="N85" s="79"/>
+      <c r="O85" s="79"/>
+      <c r="P85" s="80"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
Corrected Technologies and removed values too close to an insert table in the stoch file
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_04\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11516DAD-34D7-4C6F-901A-54820CE95A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A4A2A7-3138-4BC6-AC21-5BB2FFD58D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
@@ -780,7 +779,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="230">
   <si>
     <t>~FI_T</t>
   </si>
@@ -1456,31 +1455,40 @@
     <t>YES</t>
   </si>
   <si>
-    <t>ELERNWINDOFF15</t>
-  </si>
-  <si>
-    <t>ELERNWINDOFF25</t>
-  </si>
-  <si>
-    <t>ELERNWINDOFF35</t>
-  </si>
-  <si>
     <t>ELERNWINDOFF45</t>
   </si>
   <si>
-    <t>Power Plants New - Wind Offshore 15 m</t>
-  </si>
-  <si>
-    <t>Power Plants New - Wind Offshore 25 m</t>
-  </si>
-  <si>
-    <t>Power Plants New - Wind Offshore 35 m</t>
-  </si>
-  <si>
-    <t>Power Plants New - Wind Offshore 45 m</t>
-  </si>
-  <si>
     <t>*ENV_ACT</t>
+  </si>
+  <si>
+    <t>ELCWINOFF45</t>
+  </si>
+  <si>
+    <t>ELERNWINDOFF8</t>
+  </si>
+  <si>
+    <t>ELERNWINDOFF20</t>
+  </si>
+  <si>
+    <t>ELERNWINDOFF30</t>
+  </si>
+  <si>
+    <t>ELCWINOFF8</t>
+  </si>
+  <si>
+    <t>ELCWINOFF20</t>
+  </si>
+  <si>
+    <t>ELCWINOFF30</t>
+  </si>
+  <si>
+    <t>Power Plants New - Wind Offshore 8,4 WTG</t>
+  </si>
+  <si>
+    <t>Power Plants New - Wind Offshore 20 WTG</t>
+  </si>
+  <si>
+    <t>Power Plants New - Wind Offshore 30 WTG</t>
   </si>
 </sst>
 </file>
@@ -1493,10 +1501,17 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1889,222 +1904,233 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="37" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="37"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="47"/>
-    <xf numFmtId="2" fontId="1" fillId="10" borderId="0" xfId="49" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="37" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="37"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="10" borderId="0" xfId="49" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="51" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" xfId="51" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="51" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="51" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" xfId="51" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" xfId="51" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="51" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="51" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="53">
     <cellStyle name="20 % - Farve5" xfId="1" builtinId="46"/>
     <cellStyle name="20 % - Farve5 2" xfId="21" xr:uid="{A0E445DD-DB75-4F07-98F7-EA4A3CF45A39}"/>
     <cellStyle name="20 % - Farve5 3" xfId="38" xr:uid="{8A40DF18-D052-4DB8-B40C-15BAC6E6B7D7}"/>
     <cellStyle name="20 % - Farve5 4" xfId="48" xr:uid="{BA84CF23-2043-4E52-89AD-E947642EEB2E}"/>
     <cellStyle name="20 % - Farve5 5" xfId="50" xr:uid="{66152348-0630-41BB-A0D0-D003EB9CAD6B}"/>
+    <cellStyle name="20 % - Farve5 6" xfId="52" xr:uid="{F2E84A5F-13F5-47BB-BEC9-CC64879C4939}"/>
     <cellStyle name="60 % - Farve2 2" xfId="22" xr:uid="{C9AC1626-ABF5-4D3D-AC98-65C9B7342771}"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Comma 2 2" xfId="23" xr:uid="{342F0051-E0EA-4BA9-AC78-716E2BD62BB9}"/>
@@ -2132,6 +2158,7 @@
     <cellStyle name="Normal 8" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Normal 8 2" xfId="25" xr:uid="{4EED7756-B081-4876-9BFC-75CEBE779579}"/>
     <cellStyle name="Normal 8 3" xfId="40" xr:uid="{05D6DDAC-C833-4036-89B1-416002114B0D}"/>
+    <cellStyle name="Normal 9" xfId="51" xr:uid="{E3D3CD42-8373-46A8-8172-4A75C48FCCBD}"/>
     <cellStyle name="Normal 9 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normale_B2020" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Percent 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
@@ -3332,44 +3359,6 @@
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sector_Fuels_ELC"/>
-      <sheetName val="Con_ELC"/>
-      <sheetName val="Emi"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="19">
-          <cell r="C19" t="str">
-            <v>ELCWINOFF15</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20" t="str">
-            <v>ELCWINOFF25</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21" t="str">
-            <v>ELCWINOFF35</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22" t="str">
-            <v>ELCWINOFF45</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
@@ -3398,7 +3387,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -3712,10 +3701,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:AL85"/>
+  <dimension ref="A1:AL87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3981,7 +3970,7 @@
         <v>174</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="P11" s="14" t="s">
         <v>113</v>
@@ -4086,13 +4075,11 @@
       <c r="AA13" s="44"/>
     </row>
     <row r="14" spans="1:36" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B14" s="22" t="str">
-        <f>U17</f>
-        <v>ELERNWINDOFF15</v>
-      </c>
-      <c r="C14" s="22" t="str">
-        <f>[2]Sector_Fuels_ELC!$C$19</f>
-        <v>ELCWINOFF15</v>
+      <c r="B14" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>224</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>49</v>
@@ -4109,14 +4096,14 @@
       <c r="H14" s="26">
         <v>0.48</v>
       </c>
-      <c r="I14" s="85">
-        <v>1809.5</v>
-      </c>
-      <c r="J14" s="26">
-        <v>54.29</v>
-      </c>
-      <c r="K14" s="86">
-        <v>1.1399999999999999</v>
+      <c r="I14" s="86">
+        <v>1900</v>
+      </c>
+      <c r="J14" s="87">
+        <v>57</v>
+      </c>
+      <c r="K14" s="85">
+        <v>1.19</v>
       </c>
       <c r="L14" s="22">
         <v>30</v>
@@ -4159,13 +4146,11 @@
       </c>
     </row>
     <row r="15" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="22" t="str">
-        <f>U18</f>
-        <v>ELERNWINDOFF25</v>
-      </c>
-      <c r="C15" s="22" t="str">
-        <f>[2]Sector_Fuels_ELC!$C$20</f>
-        <v>ELCWINOFF25</v>
+      <c r="B15" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>225</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>49</v>
@@ -4182,14 +4167,14 @@
       <c r="H15" s="26">
         <v>0.48</v>
       </c>
-      <c r="I15" s="22">
-        <v>1900</v>
-      </c>
-      <c r="J15" s="26">
-        <v>57</v>
-      </c>
-      <c r="K15" s="86">
-        <v>1.19</v>
+      <c r="I15" s="92">
+        <v>2060</v>
+      </c>
+      <c r="J15" s="90">
+        <v>61.8</v>
+      </c>
+      <c r="K15" s="88">
+        <v>1.3755552382765401</v>
       </c>
       <c r="L15" s="22">
         <v>30</v>
@@ -4232,13 +4217,11 @@
       </c>
     </row>
     <row r="16" spans="1:36" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B16" s="22" t="str">
-        <f t="shared" ref="B16:B17" si="0">U19</f>
-        <v>ELERNWINDOFF35</v>
-      </c>
-      <c r="C16" s="22" t="str">
-        <f>[2]Sector_Fuels_ELC!$C$21</f>
-        <v>ELCWINOFF35</v>
+      <c r="B16" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>226</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>49</v>
@@ -4255,14 +4238,14 @@
       <c r="H16" s="26">
         <v>0.48</v>
       </c>
-      <c r="I16" s="22">
-        <v>1995</v>
-      </c>
-      <c r="J16" s="26">
-        <v>59.83</v>
-      </c>
-      <c r="K16" s="86">
-        <v>1.25</v>
+      <c r="I16" s="94">
+        <v>2180</v>
+      </c>
+      <c r="J16" s="91">
+        <v>65.399999999999991</v>
+      </c>
+      <c r="K16" s="89">
+        <v>1.726314157819919</v>
       </c>
       <c r="L16" s="22">
         <v>30</v>
@@ -4300,20 +4283,20 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="2:27" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>ELERNWINDOFF45</v>
+        <f>U20</f>
+        <v>ELERNWINDON</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f>[2]Sector_Fuels_ELC!$C$22</f>
-        <v>ELCWINOFF45</v>
+        <f>[2]Sector_Fuels_ELC!$C$18</f>
+        <v>ELCWINON</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="22">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="F17" s="25">
         <v>2022</v>
@@ -4322,22 +4305,23 @@
         <v>1</v>
       </c>
       <c r="H17" s="26">
-        <v>0.48</v>
+        <v>0.35</v>
       </c>
       <c r="I17" s="22">
-        <v>2071</v>
+        <v>1150</v>
       </c>
       <c r="J17" s="26">
-        <v>62.1</v>
-      </c>
-      <c r="K17" s="86">
-        <v>1.29</v>
+        <v>23</v>
+      </c>
+      <c r="K17" s="26">
+        <f>K14</f>
+        <v>1.19</v>
       </c>
       <c r="L17" s="22">
         <v>30</v>
       </c>
       <c r="M17" s="22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P17" s="22">
         <v>31.536000000000001</v>
@@ -4346,11 +4330,11 @@
         <v>1</v>
       </c>
       <c r="S17" s="44"/>
-      <c r="U17" t="s">
-        <v>218</v>
+      <c r="U17" s="93" t="s">
+        <v>221</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="W17" t="s">
         <v>52</v>
@@ -4367,12 +4351,12 @@
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="str">
-        <f>U21</f>
-        <v>ELERNWINDON</v>
+        <f>U16</f>
+        <v>ELERNWSUN01</v>
       </c>
       <c r="C18" s="22" t="str">
-        <f>[3]Sector_Fuels_ELC!$C$18</f>
-        <v>ELCWINON</v>
+        <f>[2]Sector_Fuels_ELC!$C$20</f>
+        <v>ELCSOL</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>49</v>
@@ -4387,23 +4371,22 @@
         <v>1</v>
       </c>
       <c r="H18" s="26">
-        <v>0.35</v>
-      </c>
-      <c r="I18" s="22">
-        <v>1150</v>
+        <v>0.12</v>
+      </c>
+      <c r="I18" s="26">
+        <f>450-J18</f>
+        <v>447</v>
       </c>
       <c r="J18" s="26">
-        <v>23</v>
-      </c>
-      <c r="K18" s="26">
-        <f>K14</f>
-        <v>1.1399999999999999</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K18" s="26"/>
       <c r="L18" s="22">
         <v>30</v>
       </c>
       <c r="M18" s="22">
-        <v>2</v>
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="P18" s="22">
         <v>31.536000000000001</v>
@@ -4411,11 +4394,11 @@
       <c r="Q18" s="22">
         <v>1</v>
       </c>
-      <c r="U18" t="s">
-        <v>219</v>
+      <c r="U18" s="93" t="s">
+        <v>222</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="W18" t="s">
         <v>52</v>
@@ -4430,56 +4413,58 @@
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="2:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="str">
-        <f>U16</f>
-        <v>ELERNWSUN01</v>
-      </c>
-      <c r="C19" s="22" t="str">
-        <f>[3]Sector_Fuels_ELC!$C$20</f>
-        <v>ELCSOL</v>
-      </c>
-      <c r="D19" s="22" t="s">
+    <row r="19" spans="2:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D19" s="52" t="s">
         <v>49</v>
       </c>
       <c r="E19" s="22">
         <v>2020</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="22">
         <v>2022</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="83">
+        <v>0.49</v>
+      </c>
+      <c r="H19" s="26">
         <v>1</v>
       </c>
-      <c r="H19" s="26">
-        <v>0.12</v>
-      </c>
       <c r="I19" s="26">
-        <f>450-J19</f>
-        <v>447</v>
+        <f>494.7</f>
+        <v>494.7</v>
       </c>
       <c r="J19" s="26">
-        <v>3</v>
-      </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="22">
-        <v>30</v>
+        <f>6.5</f>
+        <v>6.5</v>
+      </c>
+      <c r="K19" s="22">
+        <v>1.66</v>
+      </c>
+      <c r="L19" s="26">
+        <v>25</v>
       </c>
       <c r="M19" s="22">
         <f>1</f>
         <v>1</v>
       </c>
+      <c r="O19" s="82"/>
       <c r="P19" s="22">
         <v>31.536000000000001</v>
       </c>
       <c r="Q19" s="22">
         <v>1</v>
       </c>
-      <c r="U19" t="s">
-        <v>220</v>
+      <c r="U19" s="93" t="s">
+        <v>223</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="W19" t="s">
         <v>52</v>
@@ -4494,63 +4479,17 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="2:27" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B20" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="D20" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="22">
-        <v>2020</v>
-      </c>
-      <c r="F20" s="22">
-        <v>2022</v>
-      </c>
-      <c r="G20" s="83">
-        <v>0.49</v>
-      </c>
-      <c r="H20" s="26">
-        <v>1</v>
-      </c>
-      <c r="I20" s="26">
-        <f>494.7</f>
-        <v>494.7</v>
-      </c>
-      <c r="J20" s="26">
-        <f>6.5</f>
-        <v>6.5</v>
-      </c>
-      <c r="K20" s="22">
-        <v>1.66</v>
-      </c>
-      <c r="L20" s="26">
-        <v>25</v>
-      </c>
-      <c r="M20" s="22">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="O20" s="82"/>
-      <c r="P20" s="22">
-        <v>31.536000000000001</v>
-      </c>
-      <c r="Q20" s="22">
-        <v>1</v>
-      </c>
-      <c r="U20" t="s">
-        <v>221</v>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="U20" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="W20" t="s">
+        <v>178</v>
+      </c>
+      <c r="W20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="X20" t="s">
+      <c r="X20" s="2" t="s">
         <v>53</v>
       </c>
       <c r="Y20" t="s">
@@ -4561,19 +4500,19 @@
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="U21" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="V21" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="W21" s="2" t="s">
+      <c r="U21" s="81" t="s">
+        <v>214</v>
+      </c>
+      <c r="V21" s="81" t="s">
+        <v>213</v>
+      </c>
+      <c r="W21" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="X21" s="2" t="s">
+      <c r="X21" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Y21" s="81" t="s">
         <v>175</v>
       </c>
       <c r="AA21" s="48" t="s">
@@ -4581,24 +4520,7 @@
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="U22" s="81" t="s">
-        <v>214</v>
-      </c>
-      <c r="V22" s="81" t="s">
-        <v>213</v>
-      </c>
-      <c r="W22" s="81" t="s">
-        <v>52</v>
-      </c>
-      <c r="X22" s="81" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y22" s="81" t="s">
-        <v>175</v>
-      </c>
-      <c r="AA22" s="48" t="s">
-        <v>217</v>
-      </c>
+      <c r="AA22" s="48"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.25">
       <c r="J24" s="22">
@@ -4733,7 +4655,7 @@
         <v>ELERNWSUN02</v>
       </c>
       <c r="X44" s="22" t="str">
-        <f>[4]Sector_Fuels_ELC!$C$20</f>
+        <f>[3]Sector_Fuels_ELC!$C$20</f>
         <v>ELCSOL</v>
       </c>
       <c r="Y44" s="22" t="s">
@@ -5075,7 +4997,7 @@
         <v>195</v>
       </c>
       <c r="K67" s="72">
-        <f>K66/P20</f>
+        <f>K66/P19</f>
         <v>0.74277016742770163</v>
       </c>
       <c r="L67" s="72" t="s">
@@ -5277,7 +5199,7 @@
       <c r="O80" s="66"/>
       <c r="P80" s="67"/>
     </row>
-    <row r="81" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
       <c r="I81" s="65">
         <f>I80*1000</f>
         <v>210000000</v>
@@ -5297,7 +5219,7 @@
       <c r="O81" s="66"/>
       <c r="P81" s="67"/>
     </row>
-    <row r="82" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
       <c r="I82" s="65">
         <f>I81/10^6</f>
         <v>210</v>
@@ -5312,7 +5234,7 @@
       <c r="O82" s="66"/>
       <c r="P82" s="67"/>
     </row>
-    <row r="83" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
       <c r="I83" s="77" t="s">
         <v>208</v>
       </c>
@@ -5324,7 +5246,7 @@
       <c r="O83" s="66"/>
       <c r="P83" s="67"/>
     </row>
-    <row r="84" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
       <c r="I84" s="74" t="s">
         <v>209</v>
       </c>
@@ -5336,7 +5258,7 @@
       <c r="O84" s="72"/>
       <c r="P84" s="75"/>
     </row>
-    <row r="85" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
       <c r="I85" s="78"/>
       <c r="J85" s="79"/>
       <c r="K85" s="79"/>
@@ -5345,6 +5267,44 @@
       <c r="N85" s="79"/>
       <c r="O85" s="79"/>
       <c r="P85" s="80"/>
+    </row>
+    <row r="87" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B87" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E87" s="22">
+        <v>2015</v>
+      </c>
+      <c r="F87" s="22">
+        <v>2022</v>
+      </c>
+      <c r="G87" s="22">
+        <v>1</v>
+      </c>
+      <c r="H87" s="22">
+        <v>0.48</v>
+      </c>
+      <c r="I87" s="22">
+        <v>2071</v>
+      </c>
+      <c r="J87" s="22">
+        <v>62.1</v>
+      </c>
+      <c r="K87" s="22">
+        <v>1.29</v>
+      </c>
+      <c r="L87" s="22">
+        <v>30</v>
+      </c>
+      <c r="M87" s="22">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
Files with notes now up to date
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_04\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_models\KModel_04\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E9A263-7557-4E2C-AC40-51C67F6FD714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD543218-3EBE-4FD1-9862-0C34DD4426F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="182">
   <si>
     <t>~FI_T</t>
   </si>
@@ -445,9 +444,6 @@
     </r>
   </si>
   <si>
-    <t>ELERNWSUN02</t>
-  </si>
-  <si>
     <t>*LCOE</t>
   </si>
   <si>
@@ -580,15 +576,9 @@
     <t>YES</t>
   </si>
   <si>
-    <t>ELERNWINDOFF45</t>
-  </si>
-  <si>
     <t>*ENV_ACT</t>
   </si>
   <si>
-    <t>ELCWINOFF45</t>
-  </si>
-  <si>
     <t>ELERNWINDOFF8</t>
   </si>
   <si>
@@ -614,6 +604,9 @@
   </si>
   <si>
     <t>Power Plants New - Wind Offshore 30 WTG</t>
+  </si>
+  <si>
+    <t>Unused</t>
   </si>
 </sst>
 </file>
@@ -622,7 +615,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="\Te\x\t"/>
   </numFmts>
   <fonts count="30" x14ac:knownFonts="1">
     <font>
@@ -816,7 +809,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -866,12 +859,6 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1076,7 +1063,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1149,24 +1136,24 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="11" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyAlignment="1">
@@ -1206,10 +1193,13 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="37" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="37"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="3" fillId="10" borderId="0" xfId="49" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="51" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="51" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="37" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="51" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="51" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="53">
     <cellStyle name="20 % - Farve5" xfId="1" builtinId="46"/>
@@ -1283,241 +1273,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>75777</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>245745</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>33020</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE319AE5-1D4E-46BE-8600-7A680B439B3F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10835640" y="6369897"/>
-          <a:ext cx="7652385" cy="1466003"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Define each "new"</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>power plants (FI_Process table).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Declare technology</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> attributes (FI_T) such as INVCOST. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:endParaRPr lang="en-GB" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Existing technologies are defined in the base-year template while new fuel technologies are</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> defined here.</a:t>
-          </a:r>
-          <a:endParaRPr lang="fr-CA">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Duplicate definition should be avoided. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Vintaging ELCTNGAS00 in the FI_PROCESS setting YES cellW15 and then specifing data by year in table FI_T (column Year. In this example EFF is vintaged for periods 2006 to 2020.</a:t>
-          </a:r>
-          <a:endParaRPr lang="fr-CA">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>200393</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>158416</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>251327</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>69926</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1532,8 +1297,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="259080" y="4251960"/>
-          <a:ext cx="6278880" cy="5455920"/>
+          <a:off x="200393" y="7551153"/>
+          <a:ext cx="6481145" cy="4095826"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1569,6 +1334,16 @@
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" b="1"/>
+            <a:t>Mainly</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" b="1" baseline="0"/>
+            <a:t> personal notes are found in these boxes of texts.</a:t>
+          </a:r>
+        </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="da-DK" sz="1100"/>
@@ -1628,7 +1403,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t>O&amp;M costs are assumed constant throughout a turbines lifetime, despite the fact that we know it increases as the turbine ages. </a:t>
+            <a:t>O&amp;M costs are assumed constant throughout a turbines lifetime, despite the fact that it is known to increase as the turbine ages. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1637,7 +1412,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t>As for sun, the investment cost is also from the technology catalogue, but the price is expecting to drop every year. This should probably be considered. EIA is also estimating current costs at way more, around 450 M. Euro pr GWp. So, if it invests everything into sun, try increasing the investment price to match that. </a:t>
+            <a:t>As for sun, the investment cost is also from the technology catalogue. EIA is also estimating current costs at way more, around 450 M. Euro pr GWp. I went with the cheaper option.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1680,20 +1455,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t>Efficiency also drops across lifetime, but slowly. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="da-DK" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="da-DK" sz="1100"/>
-            <a:t>Variable costs added to the sun,</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t> for run 9 in KModel_2</a:t>
+            <a:t>Efficiency also drops across lifetime, but slowly (for sun). </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1702,16 +1464,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>386347</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>74062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>118310</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>56950</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1726,8 +1488,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8328660" y="3992880"/>
-          <a:ext cx="2956560" cy="2004060"/>
+          <a:off x="12818979" y="8683325"/>
+          <a:ext cx="2953752" cy="2068362"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1803,16 +1565,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>39036</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>18984</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>889267</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>60827</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1827,8 +1589,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12656820" y="3970020"/>
-          <a:ext cx="2255520" cy="2247900"/>
+          <a:off x="14289773" y="10887510"/>
+          <a:ext cx="2253915" cy="2341212"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2051,32 +1813,6 @@
             <v>ELCWINON</v>
           </cell>
         </row>
-        <row r="20">
-          <cell r="C20" t="str">
-            <v>ELCSOL</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Sector_Fuels_ELC"/>
-      <sheetName val="Con_ELC"/>
-      <sheetName val="Emi"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
         <row r="20">
           <cell r="C20" t="str">
             <v>ELCSOL</v>
@@ -2378,10 +2114,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:AL87"/>
+  <dimension ref="A1:AL85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2641,13 +2377,13 @@
         <v>71</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P11" s="14" t="s">
         <v>96</v>
@@ -2687,7 +2423,7 @@
         <v>97</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N12" s="16" t="s">
         <v>125</v>
@@ -2718,7 +2454,7 @@
         <v>83</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>84</v>
@@ -2753,10 +2489,10 @@
     </row>
     <row r="14" spans="1:36" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B14" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>175</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>178</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>49</v>
@@ -2779,13 +2515,13 @@
       <c r="J14" s="74">
         <v>57</v>
       </c>
-      <c r="K14" s="72">
+      <c r="K14" s="75">
         <v>1.19</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="76">
         <v>30</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="76">
         <v>4</v>
       </c>
       <c r="P14" s="22">
@@ -2824,10 +2560,10 @@
     </row>
     <row r="15" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>176</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>179</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>49</v>
@@ -2853,10 +2589,10 @@
       <c r="K15" s="73">
         <v>1.3755552382765401</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="76">
         <v>30</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="76">
         <v>4</v>
       </c>
       <c r="P15" s="22">
@@ -2895,10 +2631,10 @@
     </row>
     <row r="16" spans="1:36" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B16" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>177</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>180</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>49</v>
@@ -2924,10 +2660,10 @@
       <c r="K16" s="73">
         <v>1.726314157819919</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="76">
         <v>30</v>
       </c>
-      <c r="M16" s="22">
+      <c r="M16" s="76">
         <v>4</v>
       </c>
       <c r="P16" s="22">
@@ -2941,10 +2677,10 @@
       </c>
       <c r="T16" s="37"/>
       <c r="U16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W16" t="s">
         <v>52</v>
@@ -2953,11 +2689,11 @@
         <v>53</v>
       </c>
       <c r="Y16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Z16" s="37"/>
       <c r="AA16" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.25">
@@ -2984,20 +2720,20 @@
       <c r="H17" s="25">
         <v>0.35</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="76">
         <v>1150</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="77">
         <v>23</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="77">
         <f>K14</f>
         <v>1.19</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="76">
         <v>30</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="76">
         <v>2</v>
       </c>
       <c r="P17" s="22">
@@ -3008,10 +2744,10 @@
       </c>
       <c r="S17" s="33"/>
       <c r="U17" s="22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="W17" t="s">
         <v>52</v>
@@ -3020,10 +2756,10 @@
         <v>53</v>
       </c>
       <c r="Y17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA17" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
@@ -3050,18 +2786,18 @@
       <c r="H18" s="25">
         <v>0.12</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="77">
         <f>450-J18</f>
         <v>447</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18" s="77">
         <v>3</v>
       </c>
-      <c r="K18" s="25"/>
-      <c r="L18" s="22">
+      <c r="K18" s="77"/>
+      <c r="L18" s="76">
         <v>30</v>
       </c>
-      <c r="M18" s="22">
+      <c r="M18" s="76">
         <f>1</f>
         <v>1</v>
       </c>
@@ -3072,10 +2808,10 @@
         <v>1</v>
       </c>
       <c r="U18" s="22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="W18" t="s">
         <v>52</v>
@@ -3084,18 +2820,18 @@
         <v>53</v>
       </c>
       <c r="Y18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA18" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="2:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D19" s="39" t="s">
         <v>49</v>
@@ -3112,21 +2848,21 @@
       <c r="H19" s="25">
         <v>1</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="77">
         <f>494.7</f>
         <v>494.7</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19" s="77">
         <f>6.5</f>
         <v>6.5</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="76">
         <v>1.66</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19" s="77">
         <v>25</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="76">
         <f>1</f>
         <v>1</v>
       </c>
@@ -3138,10 +2874,10 @@
         <v>1</v>
       </c>
       <c r="U19" s="22" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="W19" t="s">
         <v>52</v>
@@ -3150,18 +2886,18 @@
         <v>53</v>
       </c>
       <c r="Y19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA19" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="U20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W20" s="2" t="s">
         <v>52</v>
@@ -3170,18 +2906,18 @@
         <v>53</v>
       </c>
       <c r="Y20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA20" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="U21" s="68" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="V21" s="68" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W21" s="68" t="s">
         <v>52</v>
@@ -3190,32 +2926,22 @@
         <v>53</v>
       </c>
       <c r="Y21" s="68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA21" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.25">
       <c r="AA22" s="37"/>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="J24" s="22">
-        <f>(57.3-50)/3</f>
-        <v>2.4333333333333322</v>
-      </c>
-    </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="I26" s="25">
-        <v>1.74</v>
-      </c>
+      <c r="I26" s="25"/>
     </row>
     <row r="27" spans="2:27" ht="14.4" x14ac:dyDescent="0.3">
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
-      <c r="I27" s="25">
-        <v>1.74</v>
-      </c>
+      <c r="I27" s="25"/>
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
       <c r="N27" s="24"/>
@@ -3226,9 +2952,7 @@
     <row r="28" spans="2:27" x14ac:dyDescent="0.25">
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
-      <c r="I28" s="25">
-        <v>1.74</v>
-      </c>
+      <c r="I28" s="25"/>
       <c r="J28" s="25"/>
       <c r="K28" s="25"/>
       <c r="N28" s="24"/>
@@ -3236,19 +2960,14 @@
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.25">
       <c r="G29" s="25"/>
-      <c r="I29" s="25">
-        <v>1.74</v>
-      </c>
+      <c r="I29" s="25"/>
       <c r="N29" s="24"/>
       <c r="R29" s="37"/>
       <c r="S29" s="37"/>
       <c r="T29" s="37"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="I30" s="25">
-        <f>0.58</f>
-        <v>0.57999999999999996</v>
-      </c>
+      <c r="I30" s="25"/>
       <c r="T30" s="37"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.25">
@@ -3327,46 +3046,18 @@
       <c r="L44" s="53"/>
       <c r="M44" s="53"/>
       <c r="N44" s="54"/>
-      <c r="W44" s="22" t="str">
-        <f>W45</f>
-        <v>ELERNWSUN02</v>
-      </c>
-      <c r="X44" s="22" t="str">
-        <f>[3]Sector_Fuels_ELC!$C$20</f>
-        <v>ELCSOL</v>
-      </c>
-      <c r="Y44" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z44" s="22">
-        <v>2015</v>
-      </c>
-      <c r="AA44" s="22">
-        <v>2022</v>
-      </c>
-      <c r="AB44" s="25">
-        <v>1</v>
-      </c>
-      <c r="AC44" s="25">
-        <v>0.3</v>
-      </c>
-      <c r="AD44" s="22">
-        <v>450</v>
-      </c>
-      <c r="AE44" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="AF44" s="25">
-        <f>0.5</f>
-        <v>0.5</v>
-      </c>
-      <c r="AG44" s="22">
-        <v>25</v>
-      </c>
-      <c r="AH44" s="22">
-        <f>1</f>
-        <v>1</v>
-      </c>
+      <c r="W44" s="22"/>
+      <c r="X44" s="22"/>
+      <c r="Y44" s="22"/>
+      <c r="Z44" s="22"/>
+      <c r="AA44" s="22"/>
+      <c r="AB44" s="25"/>
+      <c r="AC44" s="25"/>
+      <c r="AD44" s="22"/>
+      <c r="AE44" s="22"/>
+      <c r="AF44" s="25"/>
+      <c r="AG44" s="22"/>
+      <c r="AH44" s="22"/>
       <c r="AI44" s="22"/>
       <c r="AJ44" s="22"/>
       <c r="AK44" s="22">
@@ -3388,21 +3079,8 @@
       <c r="L45" s="53"/>
       <c r="M45" s="53"/>
       <c r="N45" s="54"/>
-      <c r="W45" t="s">
-        <v>127</v>
-      </c>
-      <c r="X45" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y45" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z45" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA45" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="X45" s="2"/>
+      <c r="AA45" s="2"/>
       <c r="AC45" s="37"/>
     </row>
     <row r="46" spans="9:38" x14ac:dyDescent="0.25">
@@ -3494,12 +3172,12 @@
     </row>
     <row r="57" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I57" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I58" s="49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J58" s="50"/>
       <c r="K58" s="50"/>
@@ -3511,11 +3189,11 @@
     </row>
     <row r="59" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I59" s="58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J59" s="59"/>
       <c r="K59" s="60" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L59" s="59"/>
       <c r="M59" s="59"/>
@@ -3538,7 +3216,7 @@
       </c>
       <c r="M60" s="53"/>
       <c r="N60" s="53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O60" s="53"/>
       <c r="P60" s="54"/>
@@ -3560,7 +3238,7 @@
       </c>
       <c r="M61" s="53"/>
       <c r="N61" s="53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O61" s="53"/>
       <c r="P61" s="54"/>
@@ -3587,11 +3265,11 @@
     </row>
     <row r="63" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I63" s="58" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J63" s="59"/>
       <c r="K63" s="60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L63" s="59"/>
       <c r="M63" s="59"/>
@@ -3605,18 +3283,18 @@
         <v>81</v>
       </c>
       <c r="J64" s="59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K64" s="59">
         <f>23424</f>
         <v>23424</v>
       </c>
       <c r="L64" s="59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M64" s="59"/>
       <c r="N64" s="53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O64" s="53"/>
       <c r="P64" s="54"/>
@@ -3627,18 +3305,18 @@
         <v>71.05263157894737</v>
       </c>
       <c r="J65" s="59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K65" s="59">
         <f>K64/10^6</f>
         <v>2.3424E-2</v>
       </c>
       <c r="L65" s="59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M65" s="59"/>
       <c r="N65" s="53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O65" s="53"/>
       <c r="P65" s="54"/>
@@ -3649,18 +3327,18 @@
         <v>71.05263157894737</v>
       </c>
       <c r="J66" s="59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K66" s="59">
         <f>K65*1000</f>
         <v>23.423999999999999</v>
       </c>
       <c r="L66" s="59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M66" s="59"/>
       <c r="N66" s="53" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O66" s="53"/>
       <c r="P66" s="54"/>
@@ -3671,34 +3349,34 @@
         <v>2.2530641672674836</v>
       </c>
       <c r="J67" s="59" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K67" s="59">
         <f>K66/P19</f>
         <v>0.74277016742770163</v>
       </c>
       <c r="L67" s="59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M67" s="59"/>
       <c r="N67" s="53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O67" s="53"/>
       <c r="P67" s="54"/>
     </row>
     <row r="68" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I68" s="58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J68" s="59"/>
       <c r="K68" s="60" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L68" s="59"/>
       <c r="M68" s="59"/>
       <c r="N68" s="59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O68" s="59"/>
       <c r="P68" s="62">
@@ -3799,7 +3477,7 @@
         <v>118</v>
       </c>
       <c r="K76" s="53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L76" s="53"/>
       <c r="M76" s="53"/>
@@ -3809,11 +3487,11 @@
     </row>
     <row r="77" spans="9:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I77" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J77" s="59"/>
       <c r="K77" s="59" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L77" s="59"/>
       <c r="M77" s="59"/>
@@ -3829,7 +3507,7 @@
         <v>120</v>
       </c>
       <c r="K78" s="53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L78" s="53"/>
       <c r="M78" s="53"/>
@@ -3846,7 +3524,7 @@
         <v>121</v>
       </c>
       <c r="K79" s="63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L79" s="53"/>
       <c r="M79" s="53"/>
@@ -3867,16 +3545,16 @@
         <v>0.45</v>
       </c>
       <c r="L80" s="53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M80" s="53"/>
       <c r="N80" s="53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O80" s="53"/>
       <c r="P80" s="54"/>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I81" s="52">
         <f>I80*1000</f>
         <v>210000000</v>
@@ -3896,7 +3574,7 @@
       <c r="O81" s="53"/>
       <c r="P81" s="54"/>
     </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I82" s="52">
         <f>I81/10^6</f>
         <v>210</v>
@@ -3911,9 +3589,9 @@
       <c r="O82" s="53"/>
       <c r="P82" s="54"/>
     </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I83" s="64" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J83" s="53"/>
       <c r="K83" s="53"/>
@@ -3923,9 +3601,9 @@
       <c r="O83" s="53"/>
       <c r="P83" s="54"/>
     </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I84" s="61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J84" s="59"/>
       <c r="K84" s="59"/>
@@ -3935,7 +3613,7 @@
       <c r="O84" s="59"/>
       <c r="P84" s="62"/>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I85" s="65"/>
       <c r="J85" s="66"/>
       <c r="K85" s="66"/>
@@ -3944,44 +3622,6 @@
       <c r="N85" s="66"/>
       <c r="O85" s="66"/>
       <c r="P85" s="67"/>
-    </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B87" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="D87" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E87" s="22">
-        <v>2015</v>
-      </c>
-      <c r="F87" s="22">
-        <v>2022</v>
-      </c>
-      <c r="G87" s="22">
-        <v>1</v>
-      </c>
-      <c r="H87" s="22">
-        <v>0.48</v>
-      </c>
-      <c r="I87" s="22">
-        <v>2071</v>
-      </c>
-      <c r="J87" s="22">
-        <v>62.1</v>
-      </c>
-      <c r="K87" s="22">
-        <v>1.29</v>
-      </c>
-      <c r="L87" s="22">
-        <v>30</v>
-      </c>
-      <c r="M87" s="22">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -3997,7 +3637,7 @@
   <dimension ref="B1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4142,6 +3782,9 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="O5" s="28"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
@@ -4353,9 +3996,7 @@
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
-      <c r="I11" s="45">
-        <v>6</v>
-      </c>
+      <c r="I11" s="45"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>

</xml_diff>